<commit_message>
prod smoke test debugging
</commit_message>
<xml_diff>
--- a/Data Files/prodMSRPs.xlsx
+++ b/Data Files/prodMSRPs.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10509"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zsmith/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zsmith\Desktop\katalon_lexc\katalon_lexc_msrp\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1206DDCD-DA0E-D146-9F1D-CBF7C100383D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="13200"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="98">
   <si>
     <t>RC 300 RWD</t>
   </si>
@@ -324,7 +323,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
@@ -649,21 +648,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" customWidth="1"/>
     <col min="4" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>88</v>
       </c>
@@ -680,7 +679,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>9202</v>
       </c>
@@ -697,7 +696,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>9203</v>
       </c>
@@ -714,7 +713,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>9206</v>
       </c>
@@ -731,7 +730,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>9207</v>
       </c>
@@ -748,7 +747,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>9212</v>
       </c>
@@ -765,7 +764,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>9213</v>
       </c>
@@ -782,7 +781,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>9216</v>
       </c>
@@ -799,7 +798,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9217</v>
       </c>
@@ -816,7 +815,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9000</v>
       </c>
@@ -833,7 +832,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9002</v>
       </c>
@@ -850,7 +849,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9004</v>
       </c>
@@ -867,7 +866,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9040</v>
       </c>
@@ -884,7 +883,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>9042</v>
       </c>
@@ -901,7 +900,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>9044</v>
       </c>
@@ -918,7 +917,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>9005</v>
       </c>
@@ -935,7 +934,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>9502</v>
       </c>
@@ -952,7 +951,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -969,7 +968,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>9506</v>
       </c>
@@ -986,7 +985,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1003,7 +1002,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>9510</v>
       </c>
@@ -1020,7 +1019,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1037,7 +1036,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>9516</v>
       </c>
@@ -1054,7 +1053,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -1071,7 +1070,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -1085,7 +1084,7 @@
         <v>45200</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -1099,7 +1098,7 @@
         <v>47250</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -1113,7 +1112,7 @@
         <v>49415</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -1127,7 +1126,7 @@
         <v>50155</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>9700</v>
       </c>
@@ -1138,13 +1137,13 @@
         <v>2020</v>
       </c>
       <c r="D29" s="2">
-        <v>53000</v>
+        <v>53100</v>
       </c>
       <c r="E29" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -1155,13 +1154,13 @@
         <v>2020</v>
       </c>
       <c r="D30" s="2">
-        <v>55790</v>
+        <v>55890</v>
       </c>
       <c r="E30" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>9710</v>
       </c>
@@ -1172,13 +1171,13 @@
         <v>2020</v>
       </c>
       <c r="D31" s="2">
-        <v>64265</v>
+        <v>64365</v>
       </c>
       <c r="E31" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>9625</v>
       </c>
@@ -1189,13 +1188,13 @@
         <v>2020</v>
       </c>
       <c r="D32" s="2">
-        <v>86480</v>
+        <v>86580</v>
       </c>
       <c r="E32" s="1">
-        <v>1295</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>9620</v>
       </c>
@@ -1206,13 +1205,13 @@
         <v>2020</v>
       </c>
       <c r="D33" s="2">
-        <v>91480</v>
+        <v>91580</v>
       </c>
       <c r="E33" s="1">
-        <v>1295</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -1222,14 +1221,14 @@
       <c r="C34">
         <v>2020</v>
       </c>
-      <c r="D34" t="s">
-        <v>87</v>
+      <c r="D34" s="2">
+        <v>99310</v>
       </c>
       <c r="E34" s="1">
-        <v>1295</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>9820</v>
       </c>
@@ -1246,7 +1245,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>9824</v>
       </c>
@@ -1263,7 +1262,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>9830</v>
       </c>
@@ -1280,7 +1279,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>9834</v>
       </c>
@@ -1297,7 +1296,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>9821</v>
       </c>
@@ -1314,7 +1313,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>9825</v>
       </c>
@@ -1331,7 +1330,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>9844</v>
       </c>
@@ -1348,7 +1347,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>9845</v>
       </c>
@@ -1365,7 +1364,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>9846</v>
       </c>
@@ -1382,7 +1381,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>51</v>
       </c>
@@ -1399,7 +1398,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>9120</v>
       </c>
@@ -1416,7 +1415,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>9126</v>
       </c>
@@ -1433,7 +1432,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>9122</v>
       </c>
@@ -1450,7 +1449,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>9128</v>
       </c>
@@ -1467,7 +1466,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>9140</v>
       </c>
@@ -1484,7 +1483,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>9146</v>
       </c>
@@ -1501,7 +1500,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>59</v>
       </c>
@@ -1518,7 +1517,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>59</v>
       </c>
@@ -1535,7 +1534,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>9225</v>
       </c>
@@ -1552,7 +1551,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>9226</v>
       </c>
@@ -1569,7 +1568,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>9420</v>
       </c>
@@ -1586,7 +1585,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>9424</v>
       </c>
@@ -1603,7 +1602,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>9430</v>
       </c>
@@ -1620,7 +1619,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>9434</v>
       </c>
@@ -1637,7 +1636,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>9422</v>
       </c>
@@ -1654,7 +1653,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>9426</v>
       </c>
@@ -1671,7 +1670,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>9444</v>
       </c>
@@ -1688,7 +1687,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>9454</v>
       </c>
@@ -1705,7 +1704,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>9446</v>
       </c>
@@ -1722,7 +1721,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>9301</v>
       </c>
@@ -1739,7 +1738,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>9313</v>
       </c>
@@ -1756,7 +1755,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>9300</v>
       </c>
@@ -1773,7 +1772,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>9306</v>
       </c>
@@ -1790,7 +1789,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>9314</v>
       </c>
@@ -1807,7 +1806,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>9316</v>
       </c>
@@ -1824,7 +1823,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>9260</v>
       </c>
@@ -1841,7 +1840,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>9264</v>
       </c>
@@ -1858,7 +1857,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>9262</v>
       </c>
@@ -1875,7 +1874,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>9720</v>
       </c>
@@ -1892,7 +1891,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>9724</v>
       </c>
@@ -1909,7 +1908,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>9732</v>
       </c>
@@ -1926,7 +1925,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>9736</v>
       </c>
@@ -1943,7 +1942,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>9722</v>
       </c>
@@ -1960,7 +1959,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>9738</v>
       </c>
@@ -1977,7 +1976,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>9335</v>
       </c>
@@ -1994,7 +1993,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>95</v>
       </c>

</xml_diff>

<commit_message>
lx compare msrp activation
</commit_message>
<xml_diff>
--- a/Data Files/prodMSRPs.xlsx
+++ b/Data Files/prodMSRPs.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10509"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zsmith/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zsmith\Desktop\katalon_lexc\katalon_lexc_msrp\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1206DDCD-DA0E-D146-9F1D-CBF7C100383D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="13200"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="98">
   <si>
     <t>RC 300 RWD</t>
   </si>
@@ -324,7 +323,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
@@ -649,21 +648,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" customWidth="1"/>
     <col min="4" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>88</v>
       </c>
@@ -680,7 +679,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>9202</v>
       </c>
@@ -697,7 +696,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>9203</v>
       </c>
@@ -714,7 +713,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>9206</v>
       </c>
@@ -731,7 +730,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>9207</v>
       </c>
@@ -748,7 +747,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>9212</v>
       </c>
@@ -765,7 +764,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>9213</v>
       </c>
@@ -782,7 +781,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>9216</v>
       </c>
@@ -799,7 +798,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9217</v>
       </c>
@@ -816,7 +815,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9000</v>
       </c>
@@ -833,7 +832,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9002</v>
       </c>
@@ -850,7 +849,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9004</v>
       </c>
@@ -867,7 +866,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9040</v>
       </c>
@@ -884,7 +883,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>9042</v>
       </c>
@@ -901,7 +900,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>9044</v>
       </c>
@@ -918,7 +917,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>9005</v>
       </c>
@@ -935,7 +934,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>9502</v>
       </c>
@@ -952,7 +951,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -969,7 +968,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>9506</v>
       </c>
@@ -986,7 +985,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1003,7 +1002,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>9510</v>
       </c>
@@ -1020,7 +1019,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1037,7 +1036,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>9516</v>
       </c>
@@ -1054,7 +1053,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -1071,7 +1070,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -1085,7 +1084,7 @@
         <v>45200</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -1099,7 +1098,7 @@
         <v>47250</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -1113,7 +1112,7 @@
         <v>49415</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -1127,7 +1126,7 @@
         <v>50155</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>9700</v>
       </c>
@@ -1138,13 +1137,13 @@
         <v>2020</v>
       </c>
       <c r="D29" s="2">
-        <v>53000</v>
+        <v>53100</v>
       </c>
       <c r="E29" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -1155,13 +1154,13 @@
         <v>2020</v>
       </c>
       <c r="D30" s="2">
-        <v>55790</v>
+        <v>55890</v>
       </c>
       <c r="E30" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>9710</v>
       </c>
@@ -1172,13 +1171,13 @@
         <v>2020</v>
       </c>
       <c r="D31" s="2">
-        <v>64265</v>
+        <v>64365</v>
       </c>
       <c r="E31" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>9625</v>
       </c>
@@ -1189,13 +1188,13 @@
         <v>2020</v>
       </c>
       <c r="D32" s="2">
-        <v>86480</v>
+        <v>86580</v>
       </c>
       <c r="E32" s="1">
-        <v>1295</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>9620</v>
       </c>
@@ -1206,13 +1205,13 @@
         <v>2020</v>
       </c>
       <c r="D33" s="2">
-        <v>91480</v>
+        <v>91580</v>
       </c>
       <c r="E33" s="1">
-        <v>1295</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -1222,14 +1221,14 @@
       <c r="C34">
         <v>2020</v>
       </c>
-      <c r="D34" t="s">
-        <v>87</v>
+      <c r="D34" s="2">
+        <v>99310</v>
       </c>
       <c r="E34" s="1">
-        <v>1295</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>9820</v>
       </c>
@@ -1246,7 +1245,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>9824</v>
       </c>
@@ -1263,7 +1262,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>9830</v>
       </c>
@@ -1280,7 +1279,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>9834</v>
       </c>
@@ -1297,7 +1296,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>9821</v>
       </c>
@@ -1314,7 +1313,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>9825</v>
       </c>
@@ -1331,7 +1330,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>9844</v>
       </c>
@@ -1348,7 +1347,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>9845</v>
       </c>
@@ -1365,7 +1364,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>9846</v>
       </c>
@@ -1382,7 +1381,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>51</v>
       </c>
@@ -1399,7 +1398,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>9120</v>
       </c>
@@ -1416,7 +1415,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>9126</v>
       </c>
@@ -1433,7 +1432,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>9122</v>
       </c>
@@ -1450,7 +1449,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>9128</v>
       </c>
@@ -1467,7 +1466,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>9140</v>
       </c>
@@ -1484,7 +1483,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>9146</v>
       </c>
@@ -1501,7 +1500,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>59</v>
       </c>
@@ -1518,7 +1517,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>59</v>
       </c>
@@ -1535,7 +1534,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>9225</v>
       </c>
@@ -1552,7 +1551,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>9226</v>
       </c>
@@ -1569,7 +1568,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>9420</v>
       </c>
@@ -1586,7 +1585,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>9424</v>
       </c>
@@ -1603,7 +1602,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>9430</v>
       </c>
@@ -1620,7 +1619,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>9434</v>
       </c>
@@ -1637,7 +1636,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>9422</v>
       </c>
@@ -1654,7 +1653,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>9426</v>
       </c>
@@ -1671,7 +1670,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>9444</v>
       </c>
@@ -1688,7 +1687,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>9454</v>
       </c>
@@ -1705,7 +1704,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>9446</v>
       </c>
@@ -1722,7 +1721,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>9301</v>
       </c>
@@ -1739,7 +1738,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>9313</v>
       </c>
@@ -1756,7 +1755,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>9300</v>
       </c>
@@ -1773,7 +1772,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>9306</v>
       </c>
@@ -1790,7 +1789,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>9314</v>
       </c>
@@ -1807,7 +1806,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>9316</v>
       </c>
@@ -1824,7 +1823,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>9260</v>
       </c>
@@ -1841,7 +1840,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>9264</v>
       </c>
@@ -1858,7 +1857,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>9262</v>
       </c>
@@ -1875,7 +1874,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>9720</v>
       </c>
@@ -1892,7 +1891,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>9724</v>
       </c>
@@ -1909,7 +1908,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>9732</v>
       </c>
@@ -1926,7 +1925,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>9736</v>
       </c>
@@ -1943,7 +1942,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>9722</v>
       </c>
@@ -1960,7 +1959,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>9738</v>
       </c>
@@ -1977,7 +1976,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>9335</v>
       </c>
@@ -1994,7 +1993,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>95</v>
       </c>

</xml_diff>

<commit_message>
continental us message fix
</commit_message>
<xml_diff>
--- a/Data Files/prodMSRPs.xlsx
+++ b/Data Files/prodMSRPs.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10509"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zsmith/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zsmith\Desktop\katalon_lexc\katalon_lexc_msrp\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1206DDCD-DA0E-D146-9F1D-CBF7C100383D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="13200"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="98">
   <si>
     <t>RC 300 RWD</t>
   </si>
@@ -324,7 +323,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
@@ -649,21 +648,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" customWidth="1"/>
     <col min="4" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>88</v>
       </c>
@@ -680,7 +679,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>9202</v>
       </c>
@@ -697,7 +696,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>9203</v>
       </c>
@@ -714,7 +713,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>9206</v>
       </c>
@@ -731,7 +730,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>9207</v>
       </c>
@@ -748,7 +747,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>9212</v>
       </c>
@@ -765,7 +764,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>9213</v>
       </c>
@@ -782,7 +781,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>9216</v>
       </c>
@@ -799,7 +798,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9217</v>
       </c>
@@ -816,7 +815,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9000</v>
       </c>
@@ -833,7 +832,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9002</v>
       </c>
@@ -850,7 +849,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9004</v>
       </c>
@@ -867,7 +866,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9040</v>
       </c>
@@ -884,7 +883,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>9042</v>
       </c>
@@ -901,7 +900,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>9044</v>
       </c>
@@ -918,7 +917,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>9005</v>
       </c>
@@ -935,7 +934,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>9502</v>
       </c>
@@ -952,7 +951,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -969,7 +968,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>9506</v>
       </c>
@@ -986,7 +985,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1003,7 +1002,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>9510</v>
       </c>
@@ -1020,7 +1019,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1037,7 +1036,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>9516</v>
       </c>
@@ -1054,7 +1053,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -1071,7 +1070,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -1085,7 +1084,7 @@
         <v>45200</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -1099,7 +1098,7 @@
         <v>47250</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -1113,7 +1112,7 @@
         <v>49415</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -1127,7 +1126,7 @@
         <v>50155</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>9700</v>
       </c>
@@ -1138,13 +1137,13 @@
         <v>2020</v>
       </c>
       <c r="D29" s="2">
-        <v>53000</v>
+        <v>53100</v>
       </c>
       <c r="E29" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -1155,13 +1154,13 @@
         <v>2020</v>
       </c>
       <c r="D30" s="2">
-        <v>55790</v>
+        <v>55890</v>
       </c>
       <c r="E30" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>9710</v>
       </c>
@@ -1172,13 +1171,13 @@
         <v>2020</v>
       </c>
       <c r="D31" s="2">
-        <v>64265</v>
+        <v>64365</v>
       </c>
       <c r="E31" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>9625</v>
       </c>
@@ -1189,13 +1188,13 @@
         <v>2020</v>
       </c>
       <c r="D32" s="2">
-        <v>86480</v>
+        <v>86580</v>
       </c>
       <c r="E32" s="1">
-        <v>1295</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>9620</v>
       </c>
@@ -1206,13 +1205,13 @@
         <v>2020</v>
       </c>
       <c r="D33" s="2">
-        <v>91480</v>
+        <v>91580</v>
       </c>
       <c r="E33" s="1">
-        <v>1295</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -1222,14 +1221,14 @@
       <c r="C34">
         <v>2020</v>
       </c>
-      <c r="D34" t="s">
-        <v>87</v>
+      <c r="D34" s="2">
+        <v>99310</v>
       </c>
       <c r="E34" s="1">
-        <v>1295</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>9820</v>
       </c>
@@ -1246,7 +1245,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>9824</v>
       </c>
@@ -1263,7 +1262,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>9830</v>
       </c>
@@ -1280,7 +1279,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>9834</v>
       </c>
@@ -1297,7 +1296,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>9821</v>
       </c>
@@ -1314,7 +1313,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>9825</v>
       </c>
@@ -1331,7 +1330,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>9844</v>
       </c>
@@ -1348,7 +1347,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>9845</v>
       </c>
@@ -1365,7 +1364,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>9846</v>
       </c>
@@ -1382,7 +1381,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>51</v>
       </c>
@@ -1399,7 +1398,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>9120</v>
       </c>
@@ -1416,7 +1415,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>9126</v>
       </c>
@@ -1433,7 +1432,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>9122</v>
       </c>
@@ -1450,7 +1449,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>9128</v>
       </c>
@@ -1467,7 +1466,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>9140</v>
       </c>
@@ -1484,7 +1483,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>9146</v>
       </c>
@@ -1501,7 +1500,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>59</v>
       </c>
@@ -1518,7 +1517,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>59</v>
       </c>
@@ -1535,7 +1534,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>9225</v>
       </c>
@@ -1552,7 +1551,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>9226</v>
       </c>
@@ -1569,7 +1568,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>9420</v>
       </c>
@@ -1586,7 +1585,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>9424</v>
       </c>
@@ -1603,7 +1602,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>9430</v>
       </c>
@@ -1620,7 +1619,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>9434</v>
       </c>
@@ -1637,7 +1636,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>9422</v>
       </c>
@@ -1654,7 +1653,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>9426</v>
       </c>
@@ -1671,7 +1670,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>9444</v>
       </c>
@@ -1688,7 +1687,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>9454</v>
       </c>
@@ -1705,7 +1704,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>9446</v>
       </c>
@@ -1722,7 +1721,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>9301</v>
       </c>
@@ -1739,7 +1738,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>9313</v>
       </c>
@@ -1756,7 +1755,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>9300</v>
       </c>
@@ -1773,7 +1772,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>9306</v>
       </c>
@@ -1790,7 +1789,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>9314</v>
       </c>
@@ -1807,7 +1806,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>9316</v>
       </c>
@@ -1824,7 +1823,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>9260</v>
       </c>
@@ -1841,7 +1840,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>9264</v>
       </c>
@@ -1858,7 +1857,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>9262</v>
       </c>
@@ -1875,7 +1874,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>9720</v>
       </c>
@@ -1892,7 +1891,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>9724</v>
       </c>
@@ -1909,7 +1908,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>9732</v>
       </c>
@@ -1926,7 +1925,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>9736</v>
       </c>
@@ -1943,7 +1942,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>9722</v>
       </c>
@@ -1960,7 +1959,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>9738</v>
       </c>
@@ -1977,7 +1976,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>9335</v>
       </c>
@@ -1994,7 +1993,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>95</v>
       </c>

</xml_diff>

<commit_message>
generic profile name updates
</commit_message>
<xml_diff>
--- a/Data Files/prodMSRPs.xlsx
+++ b/Data Files/prodMSRPs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="124">
   <si>
     <t>RC 300 RWD</t>
   </si>
@@ -215,9 +215,6 @@
     <t>RC F</t>
   </si>
   <si>
-    <t>RC F TRACK</t>
-  </si>
-  <si>
     <t>RX 350 FWD</t>
   </si>
   <si>
@@ -372,6 +369,33 @@
   </si>
   <si>
     <t>RX 350 AWD F SPORT BLACK LINE SPECIAL EDITION</t>
+  </si>
+  <si>
+    <t>9203SE</t>
+  </si>
+  <si>
+    <t>9207SE</t>
+  </si>
+  <si>
+    <t>9213SE</t>
+  </si>
+  <si>
+    <t>9217SE</t>
+  </si>
+  <si>
+    <t>RC 300 F SPORT Black Line</t>
+  </si>
+  <si>
+    <t>RC 300 AWD F SPORT Black Line</t>
+  </si>
+  <si>
+    <t>RC 350 F SPORT Black Line</t>
+  </si>
+  <si>
+    <t>RC 350 AWD F SPORT Black Line</t>
+  </si>
+  <si>
+    <t>RC F FUJI SPEEDWAY EDITION</t>
   </si>
 </sst>
 </file>
@@ -705,10 +729,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K95"/>
+  <dimension ref="A1:K98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B93" sqref="B93"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,19 +744,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" t="s">
         <v>88</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>89</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>90</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>91</v>
-      </c>
-      <c r="E1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -743,10 +767,10 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D2" s="2">
-        <v>41295</v>
+        <v>42120</v>
       </c>
       <c r="E2" s="1">
         <v>1025</v>
@@ -760,10 +784,10 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D3" s="2">
-        <v>46365</v>
+        <v>46590</v>
       </c>
       <c r="E3" s="1">
         <v>1025</v>
@@ -777,10 +801,10 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D4" s="2">
-        <v>43985</v>
+        <v>44810</v>
       </c>
       <c r="E4" s="1">
         <v>1025</v>
@@ -794,10 +818,10 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D5" s="2">
-        <v>48540</v>
+        <v>48765</v>
       </c>
       <c r="E5" s="1">
         <v>1025</v>
@@ -811,10 +835,10 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D6" s="2">
-        <v>44225</v>
+        <v>45050</v>
       </c>
       <c r="E6" s="1">
         <v>1025</v>
@@ -828,10 +852,10 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D7" s="2">
-        <v>49295</v>
+        <v>49520</v>
       </c>
       <c r="E7" s="1">
         <v>1025</v>
@@ -845,10 +869,10 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D8" s="2">
-        <v>46390</v>
+        <v>47215</v>
       </c>
       <c r="E8" s="1">
         <v>1025</v>
@@ -862,10 +886,10 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D9" s="2">
-        <v>50905</v>
+        <v>51130</v>
       </c>
       <c r="E9" s="1">
         <v>1025</v>
@@ -1425,7 +1449,7 @@
         <v>9846</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C43">
         <v>2021</v>
@@ -1598,10 +1622,10 @@
         <v>62</v>
       </c>
       <c r="C53">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D53" s="2">
-        <v>64900</v>
+        <v>65875</v>
       </c>
       <c r="E53" s="1">
         <v>1025</v>
@@ -1612,13 +1636,13 @@
         <v>9226</v>
       </c>
       <c r="B54" t="s">
-        <v>63</v>
+        <v>123</v>
       </c>
       <c r="C54">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D54" s="2">
-        <v>96800</v>
+        <v>97100</v>
       </c>
       <c r="E54" s="1">
         <v>1025</v>
@@ -1629,7 +1653,7 @@
         <v>9420</v>
       </c>
       <c r="B55" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C55">
         <v>2021</v>
@@ -1646,7 +1670,7 @@
         <v>9424</v>
       </c>
       <c r="B56" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C56">
         <v>2021</v>
@@ -1663,7 +1687,7 @@
         <v>9430</v>
       </c>
       <c r="B57" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C57">
         <v>2021</v>
@@ -1680,7 +1704,7 @@
         <v>9434</v>
       </c>
       <c r="B58" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C58">
         <v>2021</v>
@@ -1697,7 +1721,7 @@
         <v>9422</v>
       </c>
       <c r="B59" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C59">
         <v>2021</v>
@@ -1714,7 +1738,7 @@
         <v>9426</v>
       </c>
       <c r="B60" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C60">
         <v>2021</v>
@@ -1731,7 +1755,7 @@
         <v>9444</v>
       </c>
       <c r="B61" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C61">
         <v>2021</v>
@@ -1748,7 +1772,7 @@
         <v>9454</v>
       </c>
       <c r="B62" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C62">
         <v>2021</v>
@@ -1765,7 +1789,7 @@
         <v>9446</v>
       </c>
       <c r="B63" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C63">
         <v>2021</v>
@@ -1782,13 +1806,13 @@
         <v>9301</v>
       </c>
       <c r="B64" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C64">
         <v>2020</v>
       </c>
       <c r="D64" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E64" s="1">
         <v>1025</v>
@@ -1799,13 +1823,13 @@
         <v>9313</v>
       </c>
       <c r="B65" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C65">
         <v>2020</v>
       </c>
       <c r="D65" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E65" s="1">
         <v>1025</v>
@@ -1816,7 +1840,7 @@
         <v>9300</v>
       </c>
       <c r="B66" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C66">
         <v>2020</v>
@@ -1833,7 +1857,7 @@
         <v>9306</v>
       </c>
       <c r="B67" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C67">
         <v>2020</v>
@@ -1850,7 +1874,7 @@
         <v>9314</v>
       </c>
       <c r="B68" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C68">
         <v>2020</v>
@@ -1867,7 +1891,7 @@
         <v>9316</v>
       </c>
       <c r="B69" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C69">
         <v>2020</v>
@@ -1884,7 +1908,7 @@
         <v>9260</v>
       </c>
       <c r="B70" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C70">
         <v>2021</v>
@@ -1901,7 +1925,7 @@
         <v>9264</v>
       </c>
       <c r="B71" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C71">
         <v>2021</v>
@@ -1918,7 +1942,7 @@
         <v>9262</v>
       </c>
       <c r="B72" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C72">
         <v>2021</v>
@@ -1935,7 +1959,7 @@
         <v>9720</v>
       </c>
       <c r="B73" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C73">
         <v>2020</v>
@@ -1952,7 +1976,7 @@
         <v>9724</v>
       </c>
       <c r="B74" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C74">
         <v>2020</v>
@@ -1969,7 +1993,7 @@
         <v>9732</v>
       </c>
       <c r="B75" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C75">
         <v>2020</v>
@@ -1986,7 +2010,7 @@
         <v>9736</v>
       </c>
       <c r="B76" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C76">
         <v>2020</v>
@@ -2003,7 +2027,7 @@
         <v>9722</v>
       </c>
       <c r="B77" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C77">
         <v>2020</v>
@@ -2020,7 +2044,7 @@
         <v>9738</v>
       </c>
       <c r="B78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C78">
         <v>2020</v>
@@ -2037,7 +2061,7 @@
         <v>9335</v>
       </c>
       <c r="B79" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C79">
         <v>2020</v>
@@ -2051,10 +2075,10 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>94</v>
+      </c>
+      <c r="B80" t="s">
         <v>95</v>
-      </c>
-      <c r="B80" t="s">
-        <v>96</v>
       </c>
       <c r="C80">
         <v>2021</v>
@@ -2071,7 +2095,7 @@
         <v>9012</v>
       </c>
       <c r="B81" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C81">
         <v>2021</v>
@@ -2088,7 +2112,7 @@
         <v>9013</v>
       </c>
       <c r="B82" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C82">
         <v>2021</v>
@@ -2105,7 +2129,7 @@
         <v>9014</v>
       </c>
       <c r="B83" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C83">
         <v>2021</v>
@@ -2122,7 +2146,7 @@
         <v>9015</v>
       </c>
       <c r="B84" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C84">
         <v>2021</v>
@@ -2136,10 +2160,10 @@
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B85" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C85">
         <v>2021</v>
@@ -2156,7 +2180,7 @@
         <v>9423</v>
       </c>
       <c r="B86" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C86">
         <v>2021</v>
@@ -2173,7 +2197,7 @@
         <v>9427</v>
       </c>
       <c r="B87" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C87">
         <v>2021</v>
@@ -2190,7 +2214,7 @@
         <v>9447</v>
       </c>
       <c r="B88" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C88">
         <v>2021</v>
@@ -2207,7 +2231,7 @@
         <v>9432</v>
       </c>
       <c r="B89" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C89">
         <v>2021</v>
@@ -2224,7 +2248,7 @@
         <v>9436</v>
       </c>
       <c r="B90" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C90">
         <v>2021</v>
@@ -2241,7 +2265,7 @@
         <v>9457</v>
       </c>
       <c r="B91" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C91">
         <v>2021</v>
@@ -2256,10 +2280,10 @@
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B92" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C92">
         <v>2021</v>
@@ -2274,10 +2298,10 @@
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B93" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C93">
         <v>2021</v>
@@ -2292,10 +2316,10 @@
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B94" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C94">
         <v>2021</v>
@@ -2309,7 +2333,73 @@
       <c r="K94" s="1"/>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>115</v>
+      </c>
+      <c r="B95" t="s">
+        <v>119</v>
+      </c>
+      <c r="C95">
+        <v>2021</v>
+      </c>
+      <c r="D95" s="5">
+        <v>49160</v>
+      </c>
+      <c r="E95" s="1">
+        <v>1025</v>
+      </c>
       <c r="K95" s="1"/>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>116</v>
+      </c>
+      <c r="B96" t="s">
+        <v>120</v>
+      </c>
+      <c r="C96">
+        <v>2021</v>
+      </c>
+      <c r="D96" s="5">
+        <v>51335</v>
+      </c>
+      <c r="E96" s="1">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>117</v>
+      </c>
+      <c r="B97" t="s">
+        <v>121</v>
+      </c>
+      <c r="C97">
+        <v>2021</v>
+      </c>
+      <c r="D97" s="5">
+        <v>52090</v>
+      </c>
+      <c r="E97" s="1">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>118</v>
+      </c>
+      <c r="B98" t="s">
+        <v>122</v>
+      </c>
+      <c r="C98">
+        <v>2021</v>
+      </c>
+      <c r="D98" s="5">
+        <v>53700</v>
+      </c>
+      <c r="E98" s="1">
+        <v>1025</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
hp test bug fixes
</commit_message>
<xml_diff>
--- a/Data Files/prodMSRPs.xlsx
+++ b/Data Files/prodMSRPs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="124">
   <si>
     <t>RC 300 RWD</t>
   </si>
@@ -215,9 +215,6 @@
     <t>RC F</t>
   </si>
   <si>
-    <t>RC F TRACK</t>
-  </si>
-  <si>
     <t>RX 350 FWD</t>
   </si>
   <si>
@@ -374,34 +371,31 @@
     <t>RX 350 AWD F SPORT BLACK LINE SPECIAL EDITION</t>
   </si>
   <si>
-    <t>C-HR</t>
-  </si>
-  <si>
-    <t>RAV4</t>
-  </si>
-  <si>
-    <t>RAV4 Hybrid</t>
-  </si>
-  <si>
-    <t>RAV4 Prime</t>
-  </si>
-  <si>
-    <t>Venza</t>
-  </si>
-  <si>
-    <t>Highlander</t>
-  </si>
-  <si>
-    <t>Highlander Hybrid</t>
-  </si>
-  <si>
-    <t>4Runner</t>
-  </si>
-  <si>
-    <t>Sequoia</t>
-  </si>
-  <si>
-    <t>Land Cruiser</t>
+    <t>9203SE</t>
+  </si>
+  <si>
+    <t>9207SE</t>
+  </si>
+  <si>
+    <t>9213SE</t>
+  </si>
+  <si>
+    <t>9217SE</t>
+  </si>
+  <si>
+    <t>RC 300 F SPORT Black Line</t>
+  </si>
+  <si>
+    <t>RC 300 AWD F SPORT Black Line</t>
+  </si>
+  <si>
+    <t>RC 350 F SPORT Black Line</t>
+  </si>
+  <si>
+    <t>RC 350 AWD F SPORT Black Line</t>
+  </si>
+  <si>
+    <t>RC F FUJI SPEEDWAY EDITION</t>
   </si>
 </sst>
 </file>
@@ -735,10 +729,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K104"/>
+  <dimension ref="A1:K98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D102" sqref="D102"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,19 +744,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" t="s">
         <v>88</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>89</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>90</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>91</v>
-      </c>
-      <c r="E1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -773,10 +767,10 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D2" s="2">
-        <v>41295</v>
+        <v>42120</v>
       </c>
       <c r="E2" s="1">
         <v>1025</v>
@@ -790,10 +784,10 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D3" s="2">
-        <v>46365</v>
+        <v>46590</v>
       </c>
       <c r="E3" s="1">
         <v>1025</v>
@@ -807,10 +801,10 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D4" s="2">
-        <v>43985</v>
+        <v>44810</v>
       </c>
       <c r="E4" s="1">
         <v>1025</v>
@@ -824,10 +818,10 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D5" s="2">
-        <v>48540</v>
+        <v>48765</v>
       </c>
       <c r="E5" s="1">
         <v>1025</v>
@@ -841,10 +835,10 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D6" s="2">
-        <v>44225</v>
+        <v>45050</v>
       </c>
       <c r="E6" s="1">
         <v>1025</v>
@@ -858,10 +852,10 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D7" s="2">
-        <v>49295</v>
+        <v>49520</v>
       </c>
       <c r="E7" s="1">
         <v>1025</v>
@@ -875,10 +869,10 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D8" s="2">
-        <v>46390</v>
+        <v>47215</v>
       </c>
       <c r="E8" s="1">
         <v>1025</v>
@@ -892,10 +886,10 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D9" s="2">
-        <v>50905</v>
+        <v>51130</v>
       </c>
       <c r="E9" s="1">
         <v>1025</v>
@@ -1455,7 +1449,7 @@
         <v>9846</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C43">
         <v>2021</v>
@@ -1628,10 +1622,10 @@
         <v>62</v>
       </c>
       <c r="C53">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D53" s="2">
-        <v>64900</v>
+        <v>65875</v>
       </c>
       <c r="E53" s="1">
         <v>1025</v>
@@ -1642,13 +1636,13 @@
         <v>9226</v>
       </c>
       <c r="B54" t="s">
-        <v>63</v>
+        <v>123</v>
       </c>
       <c r="C54">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D54" s="2">
-        <v>96800</v>
+        <v>97100</v>
       </c>
       <c r="E54" s="1">
         <v>1025</v>
@@ -1659,7 +1653,7 @@
         <v>9420</v>
       </c>
       <c r="B55" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C55">
         <v>2021</v>
@@ -1676,7 +1670,7 @@
         <v>9424</v>
       </c>
       <c r="B56" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C56">
         <v>2021</v>
@@ -1693,7 +1687,7 @@
         <v>9430</v>
       </c>
       <c r="B57" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C57">
         <v>2021</v>
@@ -1710,7 +1704,7 @@
         <v>9434</v>
       </c>
       <c r="B58" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C58">
         <v>2021</v>
@@ -1727,7 +1721,7 @@
         <v>9422</v>
       </c>
       <c r="B59" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C59">
         <v>2021</v>
@@ -1744,7 +1738,7 @@
         <v>9426</v>
       </c>
       <c r="B60" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C60">
         <v>2021</v>
@@ -1761,7 +1755,7 @@
         <v>9444</v>
       </c>
       <c r="B61" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C61">
         <v>2021</v>
@@ -1778,7 +1772,7 @@
         <v>9454</v>
       </c>
       <c r="B62" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C62">
         <v>2021</v>
@@ -1795,7 +1789,7 @@
         <v>9446</v>
       </c>
       <c r="B63" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C63">
         <v>2021</v>
@@ -1812,13 +1806,13 @@
         <v>9301</v>
       </c>
       <c r="B64" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C64">
         <v>2020</v>
       </c>
       <c r="D64" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E64" s="1">
         <v>1025</v>
@@ -1829,13 +1823,13 @@
         <v>9313</v>
       </c>
       <c r="B65" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C65">
         <v>2020</v>
       </c>
       <c r="D65" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E65" s="1">
         <v>1025</v>
@@ -1846,7 +1840,7 @@
         <v>9300</v>
       </c>
       <c r="B66" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C66">
         <v>2020</v>
@@ -1863,7 +1857,7 @@
         <v>9306</v>
       </c>
       <c r="B67" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C67">
         <v>2020</v>
@@ -1880,7 +1874,7 @@
         <v>9314</v>
       </c>
       <c r="B68" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C68">
         <v>2020</v>
@@ -1897,7 +1891,7 @@
         <v>9316</v>
       </c>
       <c r="B69" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C69">
         <v>2020</v>
@@ -1914,7 +1908,7 @@
         <v>9260</v>
       </c>
       <c r="B70" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C70">
         <v>2021</v>
@@ -1931,7 +1925,7 @@
         <v>9264</v>
       </c>
       <c r="B71" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C71">
         <v>2021</v>
@@ -1948,7 +1942,7 @@
         <v>9262</v>
       </c>
       <c r="B72" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C72">
         <v>2021</v>
@@ -1965,7 +1959,7 @@
         <v>9720</v>
       </c>
       <c r="B73" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C73">
         <v>2020</v>
@@ -1982,7 +1976,7 @@
         <v>9724</v>
       </c>
       <c r="B74" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C74">
         <v>2020</v>
@@ -1999,7 +1993,7 @@
         <v>9732</v>
       </c>
       <c r="B75" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C75">
         <v>2020</v>
@@ -2016,7 +2010,7 @@
         <v>9736</v>
       </c>
       <c r="B76" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C76">
         <v>2020</v>
@@ -2033,7 +2027,7 @@
         <v>9722</v>
       </c>
       <c r="B77" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C77">
         <v>2020</v>
@@ -2050,7 +2044,7 @@
         <v>9738</v>
       </c>
       <c r="B78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C78">
         <v>2020</v>
@@ -2067,7 +2061,7 @@
         <v>9335</v>
       </c>
       <c r="B79" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C79">
         <v>2020</v>
@@ -2081,10 +2075,10 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>94</v>
+      </c>
+      <c r="B80" t="s">
         <v>95</v>
-      </c>
-      <c r="B80" t="s">
-        <v>96</v>
       </c>
       <c r="C80">
         <v>2021</v>
@@ -2101,7 +2095,7 @@
         <v>9012</v>
       </c>
       <c r="B81" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C81">
         <v>2021</v>
@@ -2118,7 +2112,7 @@
         <v>9013</v>
       </c>
       <c r="B82" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C82">
         <v>2021</v>
@@ -2135,7 +2129,7 @@
         <v>9014</v>
       </c>
       <c r="B83" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C83">
         <v>2021</v>
@@ -2152,7 +2146,7 @@
         <v>9015</v>
       </c>
       <c r="B84" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C84">
         <v>2021</v>
@@ -2166,10 +2160,10 @@
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B85" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C85">
         <v>2021</v>
@@ -2186,7 +2180,7 @@
         <v>9423</v>
       </c>
       <c r="B86" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C86">
         <v>2021</v>
@@ -2203,7 +2197,7 @@
         <v>9427</v>
       </c>
       <c r="B87" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C87">
         <v>2021</v>
@@ -2220,7 +2214,7 @@
         <v>9447</v>
       </c>
       <c r="B88" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C88">
         <v>2021</v>
@@ -2237,7 +2231,7 @@
         <v>9432</v>
       </c>
       <c r="B89" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C89">
         <v>2021</v>
@@ -2254,7 +2248,7 @@
         <v>9436</v>
       </c>
       <c r="B90" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C90">
         <v>2021</v>
@@ -2271,7 +2265,7 @@
         <v>9457</v>
       </c>
       <c r="B91" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C91">
         <v>2021</v>
@@ -2286,10 +2280,10 @@
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B92" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C92">
         <v>2021</v>
@@ -2304,10 +2298,10 @@
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B93" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C93">
         <v>2021</v>
@@ -2322,10 +2316,10 @@
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B94" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C94">
         <v>2021</v>
@@ -2339,114 +2333,72 @@
       <c r="K94" s="1"/>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>115</v>
+      </c>
       <c r="B95" t="s">
+        <v>119</v>
+      </c>
+      <c r="C95">
+        <v>2021</v>
+      </c>
+      <c r="D95" s="5">
+        <v>49160</v>
+      </c>
+      <c r="E95" s="1">
+        <v>1025</v>
+      </c>
+      <c r="K95" s="1"/>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>116</v>
       </c>
-      <c r="C95">
-        <v>2021</v>
-      </c>
-      <c r="D95" s="5">
-        <v>21445</v>
-      </c>
-      <c r="K95" s="1"/>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
+        <v>120</v>
+      </c>
+      <c r="C96">
+        <v>2021</v>
+      </c>
+      <c r="D96" s="5">
+        <v>51335</v>
+      </c>
+      <c r="E96" s="1">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
         <v>117</v>
       </c>
-      <c r="C96">
-        <v>2021</v>
-      </c>
-      <c r="D96" s="5">
-        <v>26050</v>
-      </c>
-    </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
+        <v>121</v>
+      </c>
+      <c r="C97">
+        <v>2021</v>
+      </c>
+      <c r="D97" s="5">
+        <v>52090</v>
+      </c>
+      <c r="E97" s="1">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>118</v>
       </c>
-      <c r="C97">
-        <v>2021</v>
-      </c>
-      <c r="D97" s="5">
-        <v>28500</v>
-      </c>
-    </row>
-    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C98">
         <v>2021</v>
       </c>
       <c r="D98" s="5">
-        <v>38100</v>
-      </c>
-    </row>
-    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B99" t="s">
-        <v>120</v>
-      </c>
-      <c r="C99">
-        <v>2021</v>
-      </c>
-      <c r="D99" s="5">
-        <v>32470</v>
-      </c>
-    </row>
-    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B100" t="s">
-        <v>121</v>
-      </c>
-      <c r="C100">
-        <v>2021</v>
-      </c>
-      <c r="D100" s="5">
-        <v>34600</v>
-      </c>
-    </row>
-    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B101" t="s">
-        <v>122</v>
-      </c>
-      <c r="C101">
-        <v>2021</v>
-      </c>
-      <c r="D101" s="5">
-        <v>38200</v>
-      </c>
-    </row>
-    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B102" t="s">
-        <v>123</v>
-      </c>
-      <c r="C102">
-        <v>2021</v>
-      </c>
-      <c r="D102" s="5">
-        <v>36340</v>
-      </c>
-    </row>
-    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B103" t="s">
-        <v>124</v>
-      </c>
-      <c r="C103">
-        <v>2021</v>
-      </c>
-      <c r="D103" s="5">
-        <v>49980</v>
-      </c>
-    </row>
-    <row r="104" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B104" t="s">
-        <v>125</v>
-      </c>
-      <c r="C104">
-        <v>2021</v>
-      </c>
-      <c r="D104" s="5">
-        <v>85415</v>
+        <v>53700</v>
+      </c>
+      <c r="E98" s="1">
+        <v>1025</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
additional design and technology tests now use module deeplinks
</commit_message>
<xml_diff>
--- a/Data Files/prodMSRPs.xlsx
+++ b/Data Files/prodMSRPs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="124">
   <si>
     <t>RC 300 RWD</t>
   </si>
@@ -71,9 +71,6 @@
     <t>ES 350 F SPORT</t>
   </si>
   <si>
-    <t>IS 300</t>
-  </si>
-  <si>
     <t>9502FK or v9502F</t>
   </si>
   <si>
@@ -89,18 +86,12 @@
     <t>IS 300 F SPORT AWD</t>
   </si>
   <si>
-    <t>IS 350 RWD</t>
-  </si>
-  <si>
     <t>9510FK or v9510F</t>
   </si>
   <si>
     <t>IS 350 F SPORT RWD</t>
   </si>
   <si>
-    <t>IS 350 AWD</t>
-  </si>
-  <si>
     <t>9516FJ or v9516F</t>
   </si>
   <si>
@@ -396,6 +387,15 @@
   </si>
   <si>
     <t>RC F FUJI SPEEDWAY EDITION</t>
+  </si>
+  <si>
+    <t>IS 300 RWD</t>
+  </si>
+  <si>
+    <t>UX 250h AWD BLACK LINE SPECIAL EDITION</t>
+  </si>
+  <si>
+    <t>COMING SOON</t>
   </si>
 </sst>
 </file>
@@ -729,7 +729,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K98"/>
+  <dimension ref="A1:K99"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="D99" sqref="D99"/>
@@ -744,19 +744,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" t="s">
         <v>87</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>88</v>
-      </c>
-      <c r="C1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E1" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1019,13 +1019,13 @@
         <v>9502</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>121</v>
       </c>
       <c r="C17">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D17" s="2">
-        <v>38560</v>
+        <v>39000</v>
       </c>
       <c r="E17" s="1">
         <v>1025</v>
@@ -1033,10 +1033,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
         <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>17</v>
       </c>
       <c r="C18">
         <v>2020</v>
@@ -1053,13 +1053,13 @@
         <v>9506</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D19" s="2">
-        <v>41010</v>
+        <v>41000</v>
       </c>
       <c r="E19" s="1">
         <v>1025</v>
@@ -1067,10 +1067,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
         <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>20</v>
       </c>
       <c r="C20">
         <v>2020</v>
@@ -1090,10 +1090,10 @@
         <v>21</v>
       </c>
       <c r="C21">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D21" s="2">
-        <v>42180</v>
+        <v>42900</v>
       </c>
       <c r="E21" s="1">
         <v>1025</v>
@@ -1101,10 +1101,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C22">
         <v>2020</v>
@@ -1121,13 +1121,13 @@
         <v>9516</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C23">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D23" s="2">
-        <v>44345</v>
+        <v>44900</v>
       </c>
       <c r="E23" s="1">
         <v>1025</v>
@@ -1135,10 +1135,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C24">
         <v>2020</v>
@@ -1152,10 +1152,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C25">
         <v>2020</v>
@@ -1166,10 +1166,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C26">
         <v>2020</v>
@@ -1180,10 +1180,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C27">
         <v>2020</v>
@@ -1194,10 +1194,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C28">
         <v>2020</v>
@@ -1211,7 +1211,7 @@
         <v>9700</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C29">
         <v>2020</v>
@@ -1225,10 +1225,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B30" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C30">
         <v>2020</v>
@@ -1245,7 +1245,7 @@
         <v>9710</v>
       </c>
       <c r="B31" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C31">
         <v>2020</v>
@@ -1262,7 +1262,7 @@
         <v>9625</v>
       </c>
       <c r="B32" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C32">
         <v>2020</v>
@@ -1279,7 +1279,7 @@
         <v>9620</v>
       </c>
       <c r="B33" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C33">
         <v>2020</v>
@@ -1293,10 +1293,10 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B34" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C34">
         <v>2020</v>
@@ -1313,7 +1313,7 @@
         <v>9820</v>
       </c>
       <c r="B35" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C35">
         <v>2021</v>
@@ -1330,7 +1330,7 @@
         <v>9824</v>
       </c>
       <c r="B36" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C36">
         <v>2021</v>
@@ -1347,7 +1347,7 @@
         <v>9830</v>
       </c>
       <c r="B37" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C37">
         <v>2021</v>
@@ -1364,7 +1364,7 @@
         <v>9834</v>
       </c>
       <c r="B38" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C38">
         <v>2021</v>
@@ -1381,7 +1381,7 @@
         <v>9821</v>
       </c>
       <c r="B39" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C39">
         <v>2021</v>
@@ -1398,7 +1398,7 @@
         <v>9825</v>
       </c>
       <c r="B40" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C40">
         <v>2021</v>
@@ -1415,7 +1415,7 @@
         <v>9844</v>
       </c>
       <c r="B41" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C41">
         <v>2021</v>
@@ -1432,7 +1432,7 @@
         <v>9845</v>
       </c>
       <c r="B42" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C42">
         <v>2021</v>
@@ -1449,7 +1449,7 @@
         <v>9846</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C43">
         <v>2021</v>
@@ -1463,10 +1463,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B44" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C44">
         <v>2020</v>
@@ -1483,7 +1483,7 @@
         <v>9120</v>
       </c>
       <c r="B45" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C45">
         <v>2020</v>
@@ -1500,7 +1500,7 @@
         <v>9126</v>
       </c>
       <c r="B46" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C46">
         <v>2020</v>
@@ -1517,7 +1517,7 @@
         <v>9122</v>
       </c>
       <c r="B47" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C47">
         <v>2020</v>
@@ -1534,7 +1534,7 @@
         <v>9128</v>
       </c>
       <c r="B48" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C48">
         <v>2020</v>
@@ -1551,7 +1551,7 @@
         <v>9140</v>
       </c>
       <c r="B49" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C49">
         <v>2020</v>
@@ -1568,7 +1568,7 @@
         <v>9146</v>
       </c>
       <c r="B50" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C50">
         <v>2020</v>
@@ -1582,10 +1582,10 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B51" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C51">
         <v>2020</v>
@@ -1599,10 +1599,10 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B52" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C52">
         <v>2020</v>
@@ -1619,7 +1619,7 @@
         <v>9225</v>
       </c>
       <c r="B53" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C53">
         <v>2021</v>
@@ -1636,7 +1636,7 @@
         <v>9226</v>
       </c>
       <c r="B54" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C54">
         <v>2021</v>
@@ -1653,7 +1653,7 @@
         <v>9420</v>
       </c>
       <c r="B55" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C55">
         <v>2021</v>
@@ -1670,7 +1670,7 @@
         <v>9424</v>
       </c>
       <c r="B56" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C56">
         <v>2021</v>
@@ -1687,7 +1687,7 @@
         <v>9430</v>
       </c>
       <c r="B57" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C57">
         <v>2021</v>
@@ -1704,7 +1704,7 @@
         <v>9434</v>
       </c>
       <c r="B58" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C58">
         <v>2021</v>
@@ -1721,7 +1721,7 @@
         <v>9422</v>
       </c>
       <c r="B59" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C59">
         <v>2021</v>
@@ -1738,7 +1738,7 @@
         <v>9426</v>
       </c>
       <c r="B60" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C60">
         <v>2021</v>
@@ -1755,7 +1755,7 @@
         <v>9444</v>
       </c>
       <c r="B61" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C61">
         <v>2021</v>
@@ -1772,7 +1772,7 @@
         <v>9454</v>
       </c>
       <c r="B62" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C62">
         <v>2021</v>
@@ -1789,7 +1789,7 @@
         <v>9446</v>
       </c>
       <c r="B63" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C63">
         <v>2021</v>
@@ -1806,13 +1806,13 @@
         <v>9301</v>
       </c>
       <c r="B64" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C64">
         <v>2020</v>
       </c>
       <c r="D64" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E64" s="1">
         <v>1025</v>
@@ -1823,13 +1823,13 @@
         <v>9313</v>
       </c>
       <c r="B65" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C65">
         <v>2020</v>
       </c>
       <c r="D65" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E65" s="1">
         <v>1025</v>
@@ -1840,7 +1840,7 @@
         <v>9300</v>
       </c>
       <c r="B66" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C66">
         <v>2020</v>
@@ -1857,7 +1857,7 @@
         <v>9306</v>
       </c>
       <c r="B67" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C67">
         <v>2020</v>
@@ -1874,7 +1874,7 @@
         <v>9314</v>
       </c>
       <c r="B68" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C68">
         <v>2020</v>
@@ -1891,7 +1891,7 @@
         <v>9316</v>
       </c>
       <c r="B69" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C69">
         <v>2020</v>
@@ -1908,7 +1908,7 @@
         <v>9260</v>
       </c>
       <c r="B70" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C70">
         <v>2021</v>
@@ -1925,7 +1925,7 @@
         <v>9264</v>
       </c>
       <c r="B71" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C71">
         <v>2021</v>
@@ -1942,7 +1942,7 @@
         <v>9262</v>
       </c>
       <c r="B72" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C72">
         <v>2021</v>
@@ -1959,13 +1959,13 @@
         <v>9720</v>
       </c>
       <c r="B73" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C73">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D73" s="3">
-        <v>32300</v>
+        <v>32900</v>
       </c>
       <c r="E73" s="1">
         <v>1025</v>
@@ -1976,13 +1976,13 @@
         <v>9724</v>
       </c>
       <c r="B74" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C74">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D74" s="3">
-        <v>37500</v>
+        <v>37600</v>
       </c>
       <c r="E74" s="1">
         <v>1025</v>
@@ -1993,13 +1993,13 @@
         <v>9732</v>
       </c>
       <c r="B75" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C75">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D75" s="3">
-        <v>34500</v>
+        <v>35100</v>
       </c>
       <c r="E75" s="1">
         <v>1025</v>
@@ -2010,13 +2010,13 @@
         <v>9736</v>
       </c>
       <c r="B76" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C76">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D76" s="3">
-        <v>39700</v>
+        <v>39800</v>
       </c>
       <c r="E76" s="1">
         <v>1025</v>
@@ -2027,13 +2027,13 @@
         <v>9722</v>
       </c>
       <c r="B77" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C77">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D77" s="3">
-        <v>34300</v>
+        <v>34900</v>
       </c>
       <c r="E77" s="1">
         <v>1025</v>
@@ -2044,13 +2044,13 @@
         <v>9738</v>
       </c>
       <c r="B78" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C78">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D78" s="3">
-        <v>36500</v>
+        <v>37100</v>
       </c>
       <c r="E78" s="1">
         <v>1025</v>
@@ -2061,7 +2061,7 @@
         <v>9335</v>
       </c>
       <c r="B79" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C79">
         <v>2020</v>
@@ -2075,10 +2075,10 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B80" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C80">
         <v>2021</v>
@@ -2095,7 +2095,7 @@
         <v>9012</v>
       </c>
       <c r="B81" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C81">
         <v>2021</v>
@@ -2112,7 +2112,7 @@
         <v>9013</v>
       </c>
       <c r="B82" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C82">
         <v>2021</v>
@@ -2129,7 +2129,7 @@
         <v>9014</v>
       </c>
       <c r="B83" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C83">
         <v>2021</v>
@@ -2146,7 +2146,7 @@
         <v>9015</v>
       </c>
       <c r="B84" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C84">
         <v>2021</v>
@@ -2160,10 +2160,10 @@
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B85" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C85">
         <v>2021</v>
@@ -2180,7 +2180,7 @@
         <v>9423</v>
       </c>
       <c r="B86" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C86">
         <v>2021</v>
@@ -2197,7 +2197,7 @@
         <v>9427</v>
       </c>
       <c r="B87" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C87">
         <v>2021</v>
@@ -2214,7 +2214,7 @@
         <v>9447</v>
       </c>
       <c r="B88" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C88">
         <v>2021</v>
@@ -2231,7 +2231,7 @@
         <v>9432</v>
       </c>
       <c r="B89" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C89">
         <v>2021</v>
@@ -2248,7 +2248,7 @@
         <v>9436</v>
       </c>
       <c r="B90" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C90">
         <v>2021</v>
@@ -2265,7 +2265,7 @@
         <v>9457</v>
       </c>
       <c r="B91" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C91">
         <v>2021</v>
@@ -2280,10 +2280,10 @@
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B92" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C92">
         <v>2021</v>
@@ -2298,10 +2298,10 @@
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
+        <v>108</v>
+      </c>
+      <c r="B93" t="s">
         <v>111</v>
-      </c>
-      <c r="B93" t="s">
-        <v>114</v>
       </c>
       <c r="C93">
         <v>2021</v>
@@ -2316,10 +2316,10 @@
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B94" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C94">
         <v>2021</v>
@@ -2334,10 +2334,10 @@
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B95" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C95">
         <v>2021</v>
@@ -2352,10 +2352,10 @@
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B96" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C96">
         <v>2021</v>
@@ -2369,10 +2369,10 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B97" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C97">
         <v>2021</v>
@@ -2386,10 +2386,10 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B98" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C98">
         <v>2021</v>
@@ -2398,6 +2398,20 @@
         <v>53700</v>
       </c>
       <c r="E98" s="1">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B99" t="s">
+        <v>122</v>
+      </c>
+      <c r="C99">
+        <v>2021</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E99" s="1">
         <v>1025</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated selectors for all design CTA and carousel buttons
</commit_message>
<xml_diff>
--- a/Data Files/prodMSRPs.xlsx
+++ b/Data Files/prodMSRPs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="124">
   <si>
     <t>RC 300 RWD</t>
   </si>
@@ -71,9 +71,6 @@
     <t>ES 350 F SPORT</t>
   </si>
   <si>
-    <t>IS 300</t>
-  </si>
-  <si>
     <t>9502FK or v9502F</t>
   </si>
   <si>
@@ -89,18 +86,12 @@
     <t>IS 300 F SPORT AWD</t>
   </si>
   <si>
-    <t>IS 350 RWD</t>
-  </si>
-  <si>
     <t>9510FK or v9510F</t>
   </si>
   <si>
     <t>IS 350 F SPORT RWD</t>
   </si>
   <si>
-    <t>IS 350 AWD</t>
-  </si>
-  <si>
     <t>9516FJ or v9516F</t>
   </si>
   <si>
@@ -215,9 +206,6 @@
     <t>RC F</t>
   </si>
   <si>
-    <t>RC F TRACK</t>
-  </si>
-  <si>
     <t>RX 350 FWD</t>
   </si>
   <si>
@@ -372,6 +360,42 @@
   </si>
   <si>
     <t>RX 350 AWD F SPORT BLACK LINE SPECIAL EDITION</t>
+  </si>
+  <si>
+    <t>9203SE</t>
+  </si>
+  <si>
+    <t>9207SE</t>
+  </si>
+  <si>
+    <t>9213SE</t>
+  </si>
+  <si>
+    <t>9217SE</t>
+  </si>
+  <si>
+    <t>RC 300 F SPORT Black Line</t>
+  </si>
+  <si>
+    <t>RC 300 AWD F SPORT Black Line</t>
+  </si>
+  <si>
+    <t>RC 350 F SPORT Black Line</t>
+  </si>
+  <si>
+    <t>RC 350 AWD F SPORT Black Line</t>
+  </si>
+  <si>
+    <t>RC F FUJI SPEEDWAY EDITION</t>
+  </si>
+  <si>
+    <t>IS 300 RWD</t>
+  </si>
+  <si>
+    <t>UX 250h AWD BLACK LINE SPECIAL EDITION</t>
+  </si>
+  <si>
+    <t>COMING SOON</t>
   </si>
 </sst>
 </file>
@@ -705,10 +729,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K95"/>
+  <dimension ref="A1:K99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B93" sqref="B93"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,19 +744,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" t="s">
         <v>88</v>
-      </c>
-      <c r="B1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -743,10 +767,10 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D2" s="2">
-        <v>41295</v>
+        <v>42120</v>
       </c>
       <c r="E2" s="1">
         <v>1025</v>
@@ -760,10 +784,10 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D3" s="2">
-        <v>46365</v>
+        <v>46590</v>
       </c>
       <c r="E3" s="1">
         <v>1025</v>
@@ -777,10 +801,10 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D4" s="2">
-        <v>43985</v>
+        <v>44810</v>
       </c>
       <c r="E4" s="1">
         <v>1025</v>
@@ -794,10 +818,10 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D5" s="2">
-        <v>48540</v>
+        <v>48765</v>
       </c>
       <c r="E5" s="1">
         <v>1025</v>
@@ -811,10 +835,10 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D6" s="2">
-        <v>44225</v>
+        <v>45050</v>
       </c>
       <c r="E6" s="1">
         <v>1025</v>
@@ -828,10 +852,10 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D7" s="2">
-        <v>49295</v>
+        <v>49520</v>
       </c>
       <c r="E7" s="1">
         <v>1025</v>
@@ -845,10 +869,10 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D8" s="2">
-        <v>46390</v>
+        <v>47215</v>
       </c>
       <c r="E8" s="1">
         <v>1025</v>
@@ -862,10 +886,10 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D9" s="2">
-        <v>50905</v>
+        <v>51130</v>
       </c>
       <c r="E9" s="1">
         <v>1025</v>
@@ -995,13 +1019,13 @@
         <v>9502</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>121</v>
       </c>
       <c r="C17">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D17" s="2">
-        <v>38560</v>
+        <v>39000</v>
       </c>
       <c r="E17" s="1">
         <v>1025</v>
@@ -1009,10 +1033,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
         <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>17</v>
       </c>
       <c r="C18">
         <v>2020</v>
@@ -1029,13 +1053,13 @@
         <v>9506</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D19" s="2">
-        <v>41010</v>
+        <v>41000</v>
       </c>
       <c r="E19" s="1">
         <v>1025</v>
@@ -1043,10 +1067,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
         <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>20</v>
       </c>
       <c r="C20">
         <v>2020</v>
@@ -1066,10 +1090,10 @@
         <v>21</v>
       </c>
       <c r="C21">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D21" s="2">
-        <v>42180</v>
+        <v>42900</v>
       </c>
       <c r="E21" s="1">
         <v>1025</v>
@@ -1077,10 +1101,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C22">
         <v>2020</v>
@@ -1097,13 +1121,13 @@
         <v>9516</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C23">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D23" s="2">
-        <v>44345</v>
+        <v>44900</v>
       </c>
       <c r="E23" s="1">
         <v>1025</v>
@@ -1111,10 +1135,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C24">
         <v>2020</v>
@@ -1128,10 +1152,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C25">
         <v>2020</v>
@@ -1142,10 +1166,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C26">
         <v>2020</v>
@@ -1156,10 +1180,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C27">
         <v>2020</v>
@@ -1170,10 +1194,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C28">
         <v>2020</v>
@@ -1187,7 +1211,7 @@
         <v>9700</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C29">
         <v>2020</v>
@@ -1201,10 +1225,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B30" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C30">
         <v>2020</v>
@@ -1221,7 +1245,7 @@
         <v>9710</v>
       </c>
       <c r="B31" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C31">
         <v>2020</v>
@@ -1238,7 +1262,7 @@
         <v>9625</v>
       </c>
       <c r="B32" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C32">
         <v>2020</v>
@@ -1255,7 +1279,7 @@
         <v>9620</v>
       </c>
       <c r="B33" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C33">
         <v>2020</v>
@@ -1269,10 +1293,10 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B34" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C34">
         <v>2020</v>
@@ -1289,7 +1313,7 @@
         <v>9820</v>
       </c>
       <c r="B35" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C35">
         <v>2021</v>
@@ -1306,7 +1330,7 @@
         <v>9824</v>
       </c>
       <c r="B36" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C36">
         <v>2021</v>
@@ -1323,7 +1347,7 @@
         <v>9830</v>
       </c>
       <c r="B37" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C37">
         <v>2021</v>
@@ -1340,7 +1364,7 @@
         <v>9834</v>
       </c>
       <c r="B38" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C38">
         <v>2021</v>
@@ -1357,7 +1381,7 @@
         <v>9821</v>
       </c>
       <c r="B39" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C39">
         <v>2021</v>
@@ -1374,7 +1398,7 @@
         <v>9825</v>
       </c>
       <c r="B40" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C40">
         <v>2021</v>
@@ -1391,7 +1415,7 @@
         <v>9844</v>
       </c>
       <c r="B41" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C41">
         <v>2021</v>
@@ -1408,7 +1432,7 @@
         <v>9845</v>
       </c>
       <c r="B42" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C42">
         <v>2021</v>
@@ -1425,7 +1449,7 @@
         <v>9846</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C43">
         <v>2021</v>
@@ -1439,10 +1463,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B44" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C44">
         <v>2020</v>
@@ -1459,7 +1483,7 @@
         <v>9120</v>
       </c>
       <c r="B45" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C45">
         <v>2020</v>
@@ -1476,7 +1500,7 @@
         <v>9126</v>
       </c>
       <c r="B46" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C46">
         <v>2020</v>
@@ -1493,7 +1517,7 @@
         <v>9122</v>
       </c>
       <c r="B47" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C47">
         <v>2020</v>
@@ -1510,7 +1534,7 @@
         <v>9128</v>
       </c>
       <c r="B48" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C48">
         <v>2020</v>
@@ -1527,7 +1551,7 @@
         <v>9140</v>
       </c>
       <c r="B49" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C49">
         <v>2020</v>
@@ -1544,7 +1568,7 @@
         <v>9146</v>
       </c>
       <c r="B50" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C50">
         <v>2020</v>
@@ -1558,10 +1582,10 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B51" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C51">
         <v>2020</v>
@@ -1575,10 +1599,10 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B52" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C52">
         <v>2020</v>
@@ -1595,13 +1619,13 @@
         <v>9225</v>
       </c>
       <c r="B53" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C53">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D53" s="2">
-        <v>64900</v>
+        <v>65875</v>
       </c>
       <c r="E53" s="1">
         <v>1025</v>
@@ -1612,13 +1636,13 @@
         <v>9226</v>
       </c>
       <c r="B54" t="s">
-        <v>63</v>
+        <v>120</v>
       </c>
       <c r="C54">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D54" s="2">
-        <v>96800</v>
+        <v>97100</v>
       </c>
       <c r="E54" s="1">
         <v>1025</v>
@@ -1629,7 +1653,7 @@
         <v>9420</v>
       </c>
       <c r="B55" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C55">
         <v>2021</v>
@@ -1646,7 +1670,7 @@
         <v>9424</v>
       </c>
       <c r="B56" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C56">
         <v>2021</v>
@@ -1663,7 +1687,7 @@
         <v>9430</v>
       </c>
       <c r="B57" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C57">
         <v>2021</v>
@@ -1680,7 +1704,7 @@
         <v>9434</v>
       </c>
       <c r="B58" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C58">
         <v>2021</v>
@@ -1697,7 +1721,7 @@
         <v>9422</v>
       </c>
       <c r="B59" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C59">
         <v>2021</v>
@@ -1714,7 +1738,7 @@
         <v>9426</v>
       </c>
       <c r="B60" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C60">
         <v>2021</v>
@@ -1731,7 +1755,7 @@
         <v>9444</v>
       </c>
       <c r="B61" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C61">
         <v>2021</v>
@@ -1748,7 +1772,7 @@
         <v>9454</v>
       </c>
       <c r="B62" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C62">
         <v>2021</v>
@@ -1765,7 +1789,7 @@
         <v>9446</v>
       </c>
       <c r="B63" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C63">
         <v>2021</v>
@@ -1782,13 +1806,13 @@
         <v>9301</v>
       </c>
       <c r="B64" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C64">
         <v>2020</v>
       </c>
       <c r="D64" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E64" s="1">
         <v>1025</v>
@@ -1799,13 +1823,13 @@
         <v>9313</v>
       </c>
       <c r="B65" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C65">
         <v>2020</v>
       </c>
       <c r="D65" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E65" s="1">
         <v>1025</v>
@@ -1816,7 +1840,7 @@
         <v>9300</v>
       </c>
       <c r="B66" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C66">
         <v>2020</v>
@@ -1833,7 +1857,7 @@
         <v>9306</v>
       </c>
       <c r="B67" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C67">
         <v>2020</v>
@@ -1850,7 +1874,7 @@
         <v>9314</v>
       </c>
       <c r="B68" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C68">
         <v>2020</v>
@@ -1867,7 +1891,7 @@
         <v>9316</v>
       </c>
       <c r="B69" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C69">
         <v>2020</v>
@@ -1884,7 +1908,7 @@
         <v>9260</v>
       </c>
       <c r="B70" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C70">
         <v>2021</v>
@@ -1901,7 +1925,7 @@
         <v>9264</v>
       </c>
       <c r="B71" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C71">
         <v>2021</v>
@@ -1918,7 +1942,7 @@
         <v>9262</v>
       </c>
       <c r="B72" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C72">
         <v>2021</v>
@@ -1935,13 +1959,13 @@
         <v>9720</v>
       </c>
       <c r="B73" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C73">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D73" s="3">
-        <v>32300</v>
+        <v>32900</v>
       </c>
       <c r="E73" s="1">
         <v>1025</v>
@@ -1952,13 +1976,13 @@
         <v>9724</v>
       </c>
       <c r="B74" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C74">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D74" s="3">
-        <v>37500</v>
+        <v>37600</v>
       </c>
       <c r="E74" s="1">
         <v>1025</v>
@@ -1969,13 +1993,13 @@
         <v>9732</v>
       </c>
       <c r="B75" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C75">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D75" s="3">
-        <v>34500</v>
+        <v>35100</v>
       </c>
       <c r="E75" s="1">
         <v>1025</v>
@@ -1986,13 +2010,13 @@
         <v>9736</v>
       </c>
       <c r="B76" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C76">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D76" s="3">
-        <v>39700</v>
+        <v>39800</v>
       </c>
       <c r="E76" s="1">
         <v>1025</v>
@@ -2003,13 +2027,13 @@
         <v>9722</v>
       </c>
       <c r="B77" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C77">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D77" s="3">
-        <v>34300</v>
+        <v>34900</v>
       </c>
       <c r="E77" s="1">
         <v>1025</v>
@@ -2020,13 +2044,13 @@
         <v>9738</v>
       </c>
       <c r="B78" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C78">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D78" s="3">
-        <v>36500</v>
+        <v>37100</v>
       </c>
       <c r="E78" s="1">
         <v>1025</v>
@@ -2037,7 +2061,7 @@
         <v>9335</v>
       </c>
       <c r="B79" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C79">
         <v>2020</v>
@@ -2051,10 +2075,10 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B80" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C80">
         <v>2021</v>
@@ -2071,7 +2095,7 @@
         <v>9012</v>
       </c>
       <c r="B81" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C81">
         <v>2021</v>
@@ -2088,7 +2112,7 @@
         <v>9013</v>
       </c>
       <c r="B82" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C82">
         <v>2021</v>
@@ -2105,7 +2129,7 @@
         <v>9014</v>
       </c>
       <c r="B83" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C83">
         <v>2021</v>
@@ -2122,7 +2146,7 @@
         <v>9015</v>
       </c>
       <c r="B84" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C84">
         <v>2021</v>
@@ -2136,10 +2160,10 @@
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B85" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C85">
         <v>2021</v>
@@ -2156,7 +2180,7 @@
         <v>9423</v>
       </c>
       <c r="B86" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C86">
         <v>2021</v>
@@ -2173,7 +2197,7 @@
         <v>9427</v>
       </c>
       <c r="B87" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C87">
         <v>2021</v>
@@ -2190,7 +2214,7 @@
         <v>9447</v>
       </c>
       <c r="B88" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C88">
         <v>2021</v>
@@ -2207,7 +2231,7 @@
         <v>9432</v>
       </c>
       <c r="B89" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C89">
         <v>2021</v>
@@ -2224,7 +2248,7 @@
         <v>9436</v>
       </c>
       <c r="B90" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C90">
         <v>2021</v>
@@ -2241,7 +2265,7 @@
         <v>9457</v>
       </c>
       <c r="B91" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C91">
         <v>2021</v>
@@ -2256,10 +2280,10 @@
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B92" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C92">
         <v>2021</v>
@@ -2274,10 +2298,10 @@
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B93" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C93">
         <v>2021</v>
@@ -2292,10 +2316,10 @@
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B94" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C94">
         <v>2021</v>
@@ -2309,7 +2333,87 @@
       <c r="K94" s="1"/>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>112</v>
+      </c>
+      <c r="B95" t="s">
+        <v>116</v>
+      </c>
+      <c r="C95">
+        <v>2021</v>
+      </c>
+      <c r="D95" s="5">
+        <v>49160</v>
+      </c>
+      <c r="E95" s="1">
+        <v>1025</v>
+      </c>
       <c r="K95" s="1"/>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>113</v>
+      </c>
+      <c r="B96" t="s">
+        <v>117</v>
+      </c>
+      <c r="C96">
+        <v>2021</v>
+      </c>
+      <c r="D96" s="5">
+        <v>51335</v>
+      </c>
+      <c r="E96" s="1">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>114</v>
+      </c>
+      <c r="B97" t="s">
+        <v>118</v>
+      </c>
+      <c r="C97">
+        <v>2021</v>
+      </c>
+      <c r="D97" s="5">
+        <v>52090</v>
+      </c>
+      <c r="E97" s="1">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>115</v>
+      </c>
+      <c r="B98" t="s">
+        <v>119</v>
+      </c>
+      <c r="C98">
+        <v>2021</v>
+      </c>
+      <c r="D98" s="5">
+        <v>53700</v>
+      </c>
+      <c r="E98" s="1">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B99" t="s">
+        <v>122</v>
+      </c>
+      <c r="C99">
+        <v>2021</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E99" s="1">
+        <v>1025</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
prod smoke test setup
</commit_message>
<xml_diff>
--- a/Data Files/prodMSRPs.xlsx
+++ b/Data Files/prodMSRPs.xlsx
@@ -731,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D99" sqref="D99"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1214,7 +1214,7 @@
         <v>32</v>
       </c>
       <c r="C29">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D29" s="2">
         <v>53100</v>
@@ -1231,10 +1231,10 @@
         <v>34</v>
       </c>
       <c r="C30">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D30" s="2">
-        <v>55890</v>
+        <v>56190</v>
       </c>
       <c r="E30" s="1">
         <v>1025</v>
@@ -1248,7 +1248,7 @@
         <v>35</v>
       </c>
       <c r="C31">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D31" s="2">
         <v>64365</v>
@@ -1486,10 +1486,10 @@
         <v>50</v>
       </c>
       <c r="C45">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D45" s="2">
-        <v>75450</v>
+        <v>76000</v>
       </c>
       <c r="E45" s="1">
         <v>1025</v>
@@ -1503,10 +1503,10 @@
         <v>51</v>
       </c>
       <c r="C46">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D46" s="2">
-        <v>78670</v>
+        <v>79250</v>
       </c>
       <c r="E46" s="1">
         <v>1025</v>
@@ -1520,10 +1520,10 @@
         <v>52</v>
       </c>
       <c r="C47">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D47" s="2">
-        <v>81450</v>
+        <v>79600</v>
       </c>
       <c r="E47" s="1">
         <v>1025</v>
@@ -1537,10 +1537,10 @@
         <v>53</v>
       </c>
       <c r="C48">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D48" s="2">
-        <v>84670</v>
+        <v>82850</v>
       </c>
       <c r="E48" s="1">
         <v>1025</v>

</xml_diff>

<commit_message>
updated with LC Inspiration price checks
</commit_message>
<xml_diff>
--- a/Data Files/prodMSRPs.xlsx
+++ b/Data Files/prodMSRPs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zsmith\Desktop\katalon_lexc\katalon_lexc_msrp\Data Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zsmith\Desktop\katalon_lexc\katalon_lexc_modelpage_lc\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="126">
   <si>
     <t>RC 300 RWD</t>
   </si>
@@ -396,6 +396,12 @@
   </si>
   <si>
     <t>COMING SOON</t>
+  </si>
+  <si>
+    <t>LC 500 INSPIRATION SERIES</t>
+  </si>
+  <si>
+    <t>9260LE</t>
   </si>
 </sst>
 </file>
@@ -729,20 +735,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K99"/>
+  <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D99" sqref="D99"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.3984375" customWidth="1"/>
     <col min="2" max="2" width="55" customWidth="1"/>
     <col min="4" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>84</v>
       </c>
@@ -759,7 +765,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>9202</v>
       </c>
@@ -770,13 +776,13 @@
         <v>2021</v>
       </c>
       <c r="D2" s="2">
-        <v>42120</v>
+        <v>42220</v>
       </c>
       <c r="E2" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>9203</v>
       </c>
@@ -787,13 +793,13 @@
         <v>2021</v>
       </c>
       <c r="D3" s="2">
-        <v>46590</v>
+        <v>46690</v>
       </c>
       <c r="E3" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>9206</v>
       </c>
@@ -804,13 +810,13 @@
         <v>2021</v>
       </c>
       <c r="D4" s="2">
-        <v>44810</v>
+        <v>44910</v>
       </c>
       <c r="E4" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>9207</v>
       </c>
@@ -821,13 +827,13 @@
         <v>2021</v>
       </c>
       <c r="D5" s="2">
-        <v>48765</v>
+        <v>48865</v>
       </c>
       <c r="E5" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>9212</v>
       </c>
@@ -838,13 +844,13 @@
         <v>2021</v>
       </c>
       <c r="D6" s="2">
-        <v>45050</v>
+        <v>45150</v>
       </c>
       <c r="E6" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>9213</v>
       </c>
@@ -855,13 +861,13 @@
         <v>2021</v>
       </c>
       <c r="D7" s="2">
-        <v>49520</v>
+        <v>49620</v>
       </c>
       <c r="E7" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>9216</v>
       </c>
@@ -872,13 +878,13 @@
         <v>2021</v>
       </c>
       <c r="D8" s="2">
-        <v>47215</v>
+        <v>47315</v>
       </c>
       <c r="E8" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>9217</v>
       </c>
@@ -889,13 +895,13 @@
         <v>2021</v>
       </c>
       <c r="D9" s="2">
-        <v>51130</v>
+        <v>51230</v>
       </c>
       <c r="E9" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>9000</v>
       </c>
@@ -906,13 +912,13 @@
         <v>2021</v>
       </c>
       <c r="D10" s="2">
-        <v>39900</v>
+        <v>40000</v>
       </c>
       <c r="E10" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>9002</v>
       </c>
@@ -923,13 +929,13 @@
         <v>2021</v>
       </c>
       <c r="D11" s="2">
-        <v>45100</v>
+        <v>45200</v>
       </c>
       <c r="E11" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>9004</v>
       </c>
@@ -940,13 +946,13 @@
         <v>2021</v>
       </c>
       <c r="D12" s="2">
-        <v>48900</v>
+        <v>49000</v>
       </c>
       <c r="E12" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>9040</v>
       </c>
@@ -957,13 +963,13 @@
         <v>2021</v>
       </c>
       <c r="D13" s="2">
-        <v>41810</v>
+        <v>41910</v>
       </c>
       <c r="E13" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>9042</v>
       </c>
@@ -974,13 +980,13 @@
         <v>2021</v>
       </c>
       <c r="D14" s="2">
-        <v>47010</v>
+        <v>47110</v>
       </c>
       <c r="E14" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>9044</v>
       </c>
@@ -991,13 +997,13 @@
         <v>2021</v>
       </c>
       <c r="D15" s="2">
-        <v>50810</v>
+        <v>50910</v>
       </c>
       <c r="E15" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>9005</v>
       </c>
@@ -1008,13 +1014,13 @@
         <v>2021</v>
       </c>
       <c r="D16" s="2">
-        <v>45700</v>
+        <v>45800</v>
       </c>
       <c r="E16" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>9502</v>
       </c>
@@ -1031,7 +1037,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1048,7 +1054,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>9506</v>
       </c>
@@ -1065,7 +1071,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1082,7 +1088,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>9510</v>
       </c>
@@ -1099,7 +1105,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1116,7 +1122,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>9516</v>
       </c>
@@ -1133,7 +1139,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1150,7 +1156,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1164,7 +1170,7 @@
         <v>45200</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1178,7 +1184,7 @@
         <v>47250</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -1192,7 +1198,7 @@
         <v>49415</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -1206,7 +1212,7 @@
         <v>50155</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>9700</v>
       </c>
@@ -1214,16 +1220,16 @@
         <v>32</v>
       </c>
       <c r="C29">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D29" s="2">
-        <v>53100</v>
+        <v>53250</v>
       </c>
       <c r="E29" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -1231,16 +1237,16 @@
         <v>34</v>
       </c>
       <c r="C30">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D30" s="2">
-        <v>55890</v>
+        <v>56340</v>
       </c>
       <c r="E30" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>9710</v>
       </c>
@@ -1248,16 +1254,16 @@
         <v>35</v>
       </c>
       <c r="C31">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D31" s="2">
-        <v>64365</v>
+        <v>64515</v>
       </c>
       <c r="E31" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>9625</v>
       </c>
@@ -1268,13 +1274,13 @@
         <v>2020</v>
       </c>
       <c r="D32" s="2">
-        <v>86580</v>
+        <v>86730</v>
       </c>
       <c r="E32" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>9620</v>
       </c>
@@ -1285,13 +1291,13 @@
         <v>2020</v>
       </c>
       <c r="D33" s="2">
-        <v>91580</v>
+        <v>91730</v>
       </c>
       <c r="E33" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -1308,7 +1314,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>9820</v>
       </c>
@@ -1319,13 +1325,13 @@
         <v>2021</v>
       </c>
       <c r="D35" s="2">
-        <v>37510</v>
+        <v>37610</v>
       </c>
       <c r="E35" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>9824</v>
       </c>
@@ -1336,13 +1342,13 @@
         <v>2021</v>
       </c>
       <c r="D36" s="2">
-        <v>38910</v>
+        <v>39010</v>
       </c>
       <c r="E36" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>9830</v>
       </c>
@@ -1353,13 +1359,13 @@
         <v>2021</v>
       </c>
       <c r="D37" s="2">
-        <v>39610</v>
+        <v>39710</v>
       </c>
       <c r="E37" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>9834</v>
       </c>
@@ -1370,13 +1376,13 @@
         <v>2021</v>
       </c>
       <c r="D38" s="2">
-        <v>41010</v>
+        <v>41110</v>
       </c>
       <c r="E38" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>9821</v>
       </c>
@@ -1387,13 +1393,13 @@
         <v>2021</v>
       </c>
       <c r="D39" s="2">
-        <v>43960</v>
+        <v>44060</v>
       </c>
       <c r="E39" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>9825</v>
       </c>
@@ -1404,13 +1410,13 @@
         <v>2021</v>
       </c>
       <c r="D40" s="2">
-        <v>45360</v>
+        <v>45460</v>
       </c>
       <c r="E40" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>9844</v>
       </c>
@@ -1421,13 +1427,13 @@
         <v>2021</v>
       </c>
       <c r="D41" s="2">
-        <v>40060</v>
+        <v>40160</v>
       </c>
       <c r="E41" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>9845</v>
       </c>
@@ -1438,13 +1444,13 @@
         <v>2021</v>
       </c>
       <c r="D42" s="2">
-        <v>46510</v>
+        <v>46610</v>
       </c>
       <c r="E42" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>9846</v>
       </c>
@@ -1455,13 +1461,13 @@
         <v>2021</v>
       </c>
       <c r="D43" s="2">
-        <v>46810</v>
+        <v>46910</v>
       </c>
       <c r="E43" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>48</v>
       </c>
@@ -1478,7 +1484,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A45">
         <v>9120</v>
       </c>
@@ -1486,16 +1492,16 @@
         <v>50</v>
       </c>
       <c r="C45">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D45" s="2">
-        <v>75450</v>
+        <v>76000</v>
       </c>
       <c r="E45" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A46">
         <v>9126</v>
       </c>
@@ -1503,16 +1509,16 @@
         <v>51</v>
       </c>
       <c r="C46">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D46" s="2">
-        <v>78670</v>
+        <v>79250</v>
       </c>
       <c r="E46" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A47">
         <v>9122</v>
       </c>
@@ -1520,16 +1526,16 @@
         <v>52</v>
       </c>
       <c r="C47">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D47" s="2">
-        <v>81450</v>
+        <v>79600</v>
       </c>
       <c r="E47" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A48">
         <v>9128</v>
       </c>
@@ -1537,16 +1543,16 @@
         <v>53</v>
       </c>
       <c r="C48">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D48" s="2">
-        <v>84670</v>
+        <v>82850</v>
       </c>
       <c r="E48" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A49">
         <v>9140</v>
       </c>
@@ -1563,7 +1569,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A50">
         <v>9146</v>
       </c>
@@ -1580,7 +1586,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>56</v>
       </c>
@@ -1597,7 +1603,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>56</v>
       </c>
@@ -1614,7 +1620,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A53">
         <v>9225</v>
       </c>
@@ -1625,13 +1631,13 @@
         <v>2021</v>
       </c>
       <c r="D53" s="2">
-        <v>65875</v>
+        <v>65975</v>
       </c>
       <c r="E53" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A54">
         <v>9226</v>
       </c>
@@ -1642,13 +1648,13 @@
         <v>2021</v>
       </c>
       <c r="D54" s="2">
-        <v>97100</v>
+        <v>97625</v>
       </c>
       <c r="E54" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A55">
         <v>9420</v>
       </c>
@@ -1659,13 +1665,13 @@
         <v>2021</v>
       </c>
       <c r="D55" s="2">
-        <v>45070</v>
+        <v>45170</v>
       </c>
       <c r="E55" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A56">
         <v>9424</v>
       </c>
@@ -1676,13 +1682,13 @@
         <v>2021</v>
       </c>
       <c r="D56" s="2">
-        <v>46470</v>
+        <v>46570</v>
       </c>
       <c r="E56" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A57">
         <v>9430</v>
       </c>
@@ -1693,13 +1699,13 @@
         <v>2021</v>
       </c>
       <c r="D57" s="2">
-        <v>47900</v>
+        <v>48000</v>
       </c>
       <c r="E57" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A58">
         <v>9434</v>
       </c>
@@ -1710,13 +1716,13 @@
         <v>2021</v>
       </c>
       <c r="D58" s="2">
-        <v>49300</v>
+        <v>49400</v>
       </c>
       <c r="E58" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A59">
         <v>9422</v>
       </c>
@@ -1727,13 +1733,13 @@
         <v>2021</v>
       </c>
       <c r="D59" s="2">
-        <v>48550</v>
+        <v>48650</v>
       </c>
       <c r="E59" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A60">
         <v>9426</v>
       </c>
@@ -1744,13 +1750,13 @@
         <v>2021</v>
       </c>
       <c r="D60" s="2">
-        <v>49950</v>
+        <v>50050</v>
       </c>
       <c r="E60" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A61">
         <v>9444</v>
       </c>
@@ -1761,13 +1767,13 @@
         <v>2021</v>
       </c>
       <c r="D61" s="2">
-        <v>47720</v>
+        <v>47820</v>
       </c>
       <c r="E61" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A62">
         <v>9454</v>
       </c>
@@ -1778,13 +1784,13 @@
         <v>2021</v>
       </c>
       <c r="D62" s="2">
-        <v>51110</v>
+        <v>51210</v>
       </c>
       <c r="E62" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A63">
         <v>9446</v>
       </c>
@@ -1795,13 +1801,13 @@
         <v>2021</v>
       </c>
       <c r="D63" s="2">
-        <v>51200</v>
+        <v>51300</v>
       </c>
       <c r="E63" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A64">
         <v>9301</v>
       </c>
@@ -1818,7 +1824,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A65">
         <v>9313</v>
       </c>
@@ -1835,7 +1841,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A66">
         <v>9300</v>
       </c>
@@ -1852,7 +1858,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A67">
         <v>9306</v>
       </c>
@@ -1869,7 +1875,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A68">
         <v>9314</v>
       </c>
@@ -1886,7 +1892,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A69">
         <v>9316</v>
       </c>
@@ -1903,7 +1909,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A70">
         <v>9260</v>
       </c>
@@ -1914,13 +1920,13 @@
         <v>2021</v>
       </c>
       <c r="D70" s="2">
-        <v>92950</v>
+        <v>93050</v>
       </c>
       <c r="E70" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A71">
         <v>9264</v>
       </c>
@@ -1931,13 +1937,13 @@
         <v>2021</v>
       </c>
       <c r="D71" s="2">
-        <v>97510</v>
+        <v>97610</v>
       </c>
       <c r="E71" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A72">
         <v>9262</v>
       </c>
@@ -1948,13 +1954,13 @@
         <v>2021</v>
       </c>
       <c r="D72" s="2">
-        <v>101000</v>
+        <v>101100</v>
       </c>
       <c r="E72" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A73">
         <v>9720</v>
       </c>
@@ -1971,7 +1977,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A74">
         <v>9724</v>
       </c>
@@ -1988,7 +1994,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A75">
         <v>9732</v>
       </c>
@@ -2005,7 +2011,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A76">
         <v>9736</v>
       </c>
@@ -2022,7 +2028,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A77">
         <v>9722</v>
       </c>
@@ -2039,7 +2045,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A78">
         <v>9738</v>
       </c>
@@ -2056,7 +2062,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A79">
         <v>9335</v>
       </c>
@@ -2073,7 +2079,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>91</v>
       </c>
@@ -2084,13 +2090,13 @@
         <v>2021</v>
       </c>
       <c r="D80" s="2">
-        <v>119800</v>
+        <v>119900</v>
       </c>
       <c r="E80" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A81">
         <v>9012</v>
       </c>
@@ -2101,13 +2107,13 @@
         <v>2021</v>
       </c>
       <c r="D81" s="5">
-        <v>39900</v>
+        <v>40000</v>
       </c>
       <c r="E81" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A82">
         <v>9013</v>
       </c>
@@ -2118,13 +2124,13 @@
         <v>2021</v>
       </c>
       <c r="D82" s="5">
-        <v>45100</v>
+        <v>45200</v>
       </c>
       <c r="E82" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A83">
         <v>9014</v>
       </c>
@@ -2135,13 +2141,13 @@
         <v>2021</v>
       </c>
       <c r="D83" s="5">
-        <v>48900</v>
+        <v>49000</v>
       </c>
       <c r="E83" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A84">
         <v>9015</v>
       </c>
@@ -2152,13 +2158,13 @@
         <v>2021</v>
       </c>
       <c r="D84" s="5">
-        <v>45700</v>
+        <v>45800</v>
       </c>
       <c r="E84" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>110</v>
       </c>
@@ -2175,7 +2181,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A86">
         <v>9423</v>
       </c>
@@ -2186,13 +2192,13 @@
         <v>2021</v>
       </c>
       <c r="D86" s="5">
-        <v>50950</v>
+        <v>51050</v>
       </c>
       <c r="E86" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A87">
         <v>9427</v>
       </c>
@@ -2203,13 +2209,13 @@
         <v>2021</v>
       </c>
       <c r="D87" s="5">
-        <v>52350</v>
+        <v>52450</v>
       </c>
       <c r="E87" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A88">
         <v>9447</v>
       </c>
@@ -2220,13 +2226,13 @@
         <v>2021</v>
       </c>
       <c r="D88" s="5">
-        <v>53520</v>
+        <v>53620</v>
       </c>
       <c r="E88" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A89">
         <v>9432</v>
       </c>
@@ -2237,13 +2243,13 @@
         <v>2021</v>
       </c>
       <c r="D89" s="5">
-        <v>53900</v>
+        <v>54000</v>
       </c>
       <c r="E89" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A90">
         <v>9436</v>
       </c>
@@ -2254,13 +2260,13 @@
         <v>2021</v>
       </c>
       <c r="D90" s="5">
-        <v>55300</v>
+        <v>55400</v>
       </c>
       <c r="E90" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A91">
         <v>9457</v>
       </c>
@@ -2271,14 +2277,14 @@
         <v>2021</v>
       </c>
       <c r="D91" s="5">
-        <v>57110</v>
+        <v>57210</v>
       </c>
       <c r="E91" s="1">
         <v>1025</v>
       </c>
       <c r="J91" s="1"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>107</v>
       </c>
@@ -2289,14 +2295,14 @@
         <v>2021</v>
       </c>
       <c r="D92" s="5">
-        <v>49235</v>
+        <v>49335</v>
       </c>
       <c r="E92" s="1">
         <v>1025</v>
       </c>
       <c r="K92" s="1"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>108</v>
       </c>
@@ -2307,14 +2313,14 @@
         <v>2021</v>
       </c>
       <c r="D93" s="5">
-        <v>50635</v>
+        <v>50735</v>
       </c>
       <c r="E93" s="1">
         <v>1025</v>
       </c>
       <c r="K93" s="1"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
         <v>109</v>
       </c>
@@ -2325,14 +2331,14 @@
         <v>2021</v>
       </c>
       <c r="D94" s="5">
-        <v>51885</v>
+        <v>51985</v>
       </c>
       <c r="E94" s="1">
         <v>1025</v>
       </c>
       <c r="K94" s="1"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>112</v>
       </c>
@@ -2343,14 +2349,14 @@
         <v>2021</v>
       </c>
       <c r="D95" s="5">
-        <v>49160</v>
+        <v>48835</v>
       </c>
       <c r="E95" s="1">
         <v>1025</v>
       </c>
       <c r="K95" s="1"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>113</v>
       </c>
@@ -2361,13 +2367,13 @@
         <v>2021</v>
       </c>
       <c r="D96" s="5">
-        <v>51335</v>
+        <v>51010</v>
       </c>
       <c r="E96" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>114</v>
       </c>
@@ -2378,13 +2384,13 @@
         <v>2021</v>
       </c>
       <c r="D97" s="5">
-        <v>52090</v>
+        <v>51765</v>
       </c>
       <c r="E97" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>115</v>
       </c>
@@ -2395,13 +2401,13 @@
         <v>2021</v>
       </c>
       <c r="D98" s="5">
-        <v>53700</v>
+        <v>53230</v>
       </c>
       <c r="E98" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B99" t="s">
         <v>122</v>
       </c>
@@ -2412,6 +2418,23 @@
         <v>123</v>
       </c>
       <c r="E99" s="1">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A100" t="s">
+        <v>125</v>
+      </c>
+      <c r="B100" t="s">
+        <v>124</v>
+      </c>
+      <c r="C100">
+        <v>2021</v>
+      </c>
+      <c r="D100" s="2">
+        <v>110420</v>
+      </c>
+      <c r="E100" s="1">
         <v>1025</v>
       </c>
     </row>

</xml_diff>

<commit_message>
compare and legacy HP tests disabled in lower environments
</commit_message>
<xml_diff>
--- a/Data Files/prodMSRPs.xlsx
+++ b/Data Files/prodMSRPs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zsmith\Desktop\katalon_lexc\katalon_lexc_msrp\Data Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zsmith\Desktop\katalon_lexc\katalon_lexc_modelpage_lc\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="126">
   <si>
     <t>RC 300 RWD</t>
   </si>
@@ -396,6 +396,12 @@
   </si>
   <si>
     <t>COMING SOON</t>
+  </si>
+  <si>
+    <t>LC 500 INSPIRATION SERIES</t>
+  </si>
+  <si>
+    <t>9260LE</t>
   </si>
 </sst>
 </file>
@@ -729,20 +735,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K99"/>
+  <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.3984375" customWidth="1"/>
     <col min="2" max="2" width="55" customWidth="1"/>
     <col min="4" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>84</v>
       </c>
@@ -759,7 +765,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>9202</v>
       </c>
@@ -770,13 +776,13 @@
         <v>2021</v>
       </c>
       <c r="D2" s="2">
-        <v>42120</v>
+        <v>42220</v>
       </c>
       <c r="E2" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>9203</v>
       </c>
@@ -787,13 +793,13 @@
         <v>2021</v>
       </c>
       <c r="D3" s="2">
-        <v>46590</v>
+        <v>46690</v>
       </c>
       <c r="E3" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>9206</v>
       </c>
@@ -804,13 +810,13 @@
         <v>2021</v>
       </c>
       <c r="D4" s="2">
-        <v>44810</v>
+        <v>44910</v>
       </c>
       <c r="E4" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>9207</v>
       </c>
@@ -821,13 +827,13 @@
         <v>2021</v>
       </c>
       <c r="D5" s="2">
-        <v>48765</v>
+        <v>48865</v>
       </c>
       <c r="E5" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>9212</v>
       </c>
@@ -838,13 +844,13 @@
         <v>2021</v>
       </c>
       <c r="D6" s="2">
-        <v>45050</v>
+        <v>45150</v>
       </c>
       <c r="E6" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>9213</v>
       </c>
@@ -855,13 +861,13 @@
         <v>2021</v>
       </c>
       <c r="D7" s="2">
-        <v>49520</v>
+        <v>49620</v>
       </c>
       <c r="E7" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>9216</v>
       </c>
@@ -872,13 +878,13 @@
         <v>2021</v>
       </c>
       <c r="D8" s="2">
-        <v>47215</v>
+        <v>47315</v>
       </c>
       <c r="E8" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>9217</v>
       </c>
@@ -889,13 +895,13 @@
         <v>2021</v>
       </c>
       <c r="D9" s="2">
-        <v>51130</v>
+        <v>51230</v>
       </c>
       <c r="E9" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>9000</v>
       </c>
@@ -906,13 +912,13 @@
         <v>2021</v>
       </c>
       <c r="D10" s="2">
-        <v>39900</v>
+        <v>40000</v>
       </c>
       <c r="E10" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>9002</v>
       </c>
@@ -923,13 +929,13 @@
         <v>2021</v>
       </c>
       <c r="D11" s="2">
-        <v>45100</v>
+        <v>45200</v>
       </c>
       <c r="E11" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>9004</v>
       </c>
@@ -940,13 +946,13 @@
         <v>2021</v>
       </c>
       <c r="D12" s="2">
-        <v>48900</v>
+        <v>49000</v>
       </c>
       <c r="E12" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>9040</v>
       </c>
@@ -957,13 +963,13 @@
         <v>2021</v>
       </c>
       <c r="D13" s="2">
-        <v>41810</v>
+        <v>41910</v>
       </c>
       <c r="E13" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>9042</v>
       </c>
@@ -974,13 +980,13 @@
         <v>2021</v>
       </c>
       <c r="D14" s="2">
-        <v>47010</v>
+        <v>47110</v>
       </c>
       <c r="E14" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>9044</v>
       </c>
@@ -991,13 +997,13 @@
         <v>2021</v>
       </c>
       <c r="D15" s="2">
-        <v>50810</v>
+        <v>50910</v>
       </c>
       <c r="E15" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>9005</v>
       </c>
@@ -1008,13 +1014,13 @@
         <v>2021</v>
       </c>
       <c r="D16" s="2">
-        <v>45700</v>
+        <v>45800</v>
       </c>
       <c r="E16" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>9502</v>
       </c>
@@ -1031,7 +1037,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1048,7 +1054,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>9506</v>
       </c>
@@ -1065,7 +1071,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1082,7 +1088,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>9510</v>
       </c>
@@ -1099,7 +1105,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1116,7 +1122,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>9516</v>
       </c>
@@ -1133,7 +1139,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1150,7 +1156,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1164,7 +1170,7 @@
         <v>45200</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1178,7 +1184,7 @@
         <v>47250</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -1192,7 +1198,7 @@
         <v>49415</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -1206,7 +1212,7 @@
         <v>50155</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>9700</v>
       </c>
@@ -1217,13 +1223,13 @@
         <v>2021</v>
       </c>
       <c r="D29" s="2">
-        <v>53100</v>
+        <v>53250</v>
       </c>
       <c r="E29" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -1234,13 +1240,13 @@
         <v>2021</v>
       </c>
       <c r="D30" s="2">
-        <v>56190</v>
+        <v>56340</v>
       </c>
       <c r="E30" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>9710</v>
       </c>
@@ -1251,13 +1257,13 @@
         <v>2021</v>
       </c>
       <c r="D31" s="2">
-        <v>64365</v>
+        <v>64515</v>
       </c>
       <c r="E31" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>9625</v>
       </c>
@@ -1268,13 +1274,13 @@
         <v>2020</v>
       </c>
       <c r="D32" s="2">
-        <v>86580</v>
+        <v>86730</v>
       </c>
       <c r="E32" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>9620</v>
       </c>
@@ -1285,13 +1291,13 @@
         <v>2020</v>
       </c>
       <c r="D33" s="2">
-        <v>91580</v>
+        <v>91730</v>
       </c>
       <c r="E33" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -1308,7 +1314,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>9820</v>
       </c>
@@ -1319,13 +1325,13 @@
         <v>2021</v>
       </c>
       <c r="D35" s="2">
-        <v>37510</v>
+        <v>37610</v>
       </c>
       <c r="E35" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>9824</v>
       </c>
@@ -1336,13 +1342,13 @@
         <v>2021</v>
       </c>
       <c r="D36" s="2">
-        <v>38910</v>
+        <v>39010</v>
       </c>
       <c r="E36" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>9830</v>
       </c>
@@ -1353,13 +1359,13 @@
         <v>2021</v>
       </c>
       <c r="D37" s="2">
-        <v>39610</v>
+        <v>39710</v>
       </c>
       <c r="E37" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>9834</v>
       </c>
@@ -1370,13 +1376,13 @@
         <v>2021</v>
       </c>
       <c r="D38" s="2">
-        <v>41010</v>
+        <v>41110</v>
       </c>
       <c r="E38" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>9821</v>
       </c>
@@ -1387,13 +1393,13 @@
         <v>2021</v>
       </c>
       <c r="D39" s="2">
-        <v>43960</v>
+        <v>44060</v>
       </c>
       <c r="E39" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>9825</v>
       </c>
@@ -1404,13 +1410,13 @@
         <v>2021</v>
       </c>
       <c r="D40" s="2">
-        <v>45360</v>
+        <v>45460</v>
       </c>
       <c r="E40" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>9844</v>
       </c>
@@ -1421,13 +1427,13 @@
         <v>2021</v>
       </c>
       <c r="D41" s="2">
-        <v>40060</v>
+        <v>40160</v>
       </c>
       <c r="E41" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>9845</v>
       </c>
@@ -1438,13 +1444,13 @@
         <v>2021</v>
       </c>
       <c r="D42" s="2">
-        <v>46510</v>
+        <v>46610</v>
       </c>
       <c r="E42" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>9846</v>
       </c>
@@ -1455,13 +1461,13 @@
         <v>2021</v>
       </c>
       <c r="D43" s="2">
-        <v>46810</v>
+        <v>46910</v>
       </c>
       <c r="E43" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>48</v>
       </c>
@@ -1478,7 +1484,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A45">
         <v>9120</v>
       </c>
@@ -1495,7 +1501,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A46">
         <v>9126</v>
       </c>
@@ -1512,7 +1518,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A47">
         <v>9122</v>
       </c>
@@ -1529,7 +1535,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A48">
         <v>9128</v>
       </c>
@@ -1546,7 +1552,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A49">
         <v>9140</v>
       </c>
@@ -1563,7 +1569,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A50">
         <v>9146</v>
       </c>
@@ -1580,7 +1586,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>56</v>
       </c>
@@ -1597,7 +1603,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>56</v>
       </c>
@@ -1614,7 +1620,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A53">
         <v>9225</v>
       </c>
@@ -1625,13 +1631,13 @@
         <v>2021</v>
       </c>
       <c r="D53" s="2">
-        <v>65875</v>
+        <v>65975</v>
       </c>
       <c r="E53" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A54">
         <v>9226</v>
       </c>
@@ -1642,13 +1648,13 @@
         <v>2021</v>
       </c>
       <c r="D54" s="2">
-        <v>97100</v>
+        <v>97625</v>
       </c>
       <c r="E54" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A55">
         <v>9420</v>
       </c>
@@ -1659,13 +1665,13 @@
         <v>2021</v>
       </c>
       <c r="D55" s="2">
-        <v>45070</v>
+        <v>45170</v>
       </c>
       <c r="E55" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A56">
         <v>9424</v>
       </c>
@@ -1676,13 +1682,13 @@
         <v>2021</v>
       </c>
       <c r="D56" s="2">
-        <v>46470</v>
+        <v>46570</v>
       </c>
       <c r="E56" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A57">
         <v>9430</v>
       </c>
@@ -1693,13 +1699,13 @@
         <v>2021</v>
       </c>
       <c r="D57" s="2">
-        <v>47900</v>
+        <v>48000</v>
       </c>
       <c r="E57" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A58">
         <v>9434</v>
       </c>
@@ -1710,13 +1716,13 @@
         <v>2021</v>
       </c>
       <c r="D58" s="2">
-        <v>49300</v>
+        <v>49400</v>
       </c>
       <c r="E58" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A59">
         <v>9422</v>
       </c>
@@ -1727,13 +1733,13 @@
         <v>2021</v>
       </c>
       <c r="D59" s="2">
-        <v>48550</v>
+        <v>48650</v>
       </c>
       <c r="E59" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A60">
         <v>9426</v>
       </c>
@@ -1744,13 +1750,13 @@
         <v>2021</v>
       </c>
       <c r="D60" s="2">
-        <v>49950</v>
+        <v>50050</v>
       </c>
       <c r="E60" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A61">
         <v>9444</v>
       </c>
@@ -1761,13 +1767,13 @@
         <v>2021</v>
       </c>
       <c r="D61" s="2">
-        <v>47720</v>
+        <v>47820</v>
       </c>
       <c r="E61" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A62">
         <v>9454</v>
       </c>
@@ -1778,13 +1784,13 @@
         <v>2021</v>
       </c>
       <c r="D62" s="2">
-        <v>51110</v>
+        <v>51210</v>
       </c>
       <c r="E62" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A63">
         <v>9446</v>
       </c>
@@ -1795,13 +1801,13 @@
         <v>2021</v>
       </c>
       <c r="D63" s="2">
-        <v>51200</v>
+        <v>51300</v>
       </c>
       <c r="E63" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A64">
         <v>9301</v>
       </c>
@@ -1818,7 +1824,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A65">
         <v>9313</v>
       </c>
@@ -1835,7 +1841,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A66">
         <v>9300</v>
       </c>
@@ -1852,7 +1858,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A67">
         <v>9306</v>
       </c>
@@ -1869,7 +1875,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A68">
         <v>9314</v>
       </c>
@@ -1886,7 +1892,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A69">
         <v>9316</v>
       </c>
@@ -1903,7 +1909,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A70">
         <v>9260</v>
       </c>
@@ -1914,13 +1920,13 @@
         <v>2021</v>
       </c>
       <c r="D70" s="2">
-        <v>92950</v>
+        <v>93050</v>
       </c>
       <c r="E70" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A71">
         <v>9264</v>
       </c>
@@ -1931,13 +1937,13 @@
         <v>2021</v>
       </c>
       <c r="D71" s="2">
-        <v>97510</v>
+        <v>97610</v>
       </c>
       <c r="E71" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A72">
         <v>9262</v>
       </c>
@@ -1948,13 +1954,13 @@
         <v>2021</v>
       </c>
       <c r="D72" s="2">
-        <v>101000</v>
+        <v>101100</v>
       </c>
       <c r="E72" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A73">
         <v>9720</v>
       </c>
@@ -1971,7 +1977,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A74">
         <v>9724</v>
       </c>
@@ -1988,7 +1994,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A75">
         <v>9732</v>
       </c>
@@ -2005,7 +2011,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A76">
         <v>9736</v>
       </c>
@@ -2022,7 +2028,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A77">
         <v>9722</v>
       </c>
@@ -2039,7 +2045,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A78">
         <v>9738</v>
       </c>
@@ -2056,7 +2062,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A79">
         <v>9335</v>
       </c>
@@ -2073,7 +2079,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>91</v>
       </c>
@@ -2084,13 +2090,13 @@
         <v>2021</v>
       </c>
       <c r="D80" s="2">
-        <v>119800</v>
+        <v>119900</v>
       </c>
       <c r="E80" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A81">
         <v>9012</v>
       </c>
@@ -2101,13 +2107,13 @@
         <v>2021</v>
       </c>
       <c r="D81" s="5">
-        <v>39900</v>
+        <v>40000</v>
       </c>
       <c r="E81" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A82">
         <v>9013</v>
       </c>
@@ -2118,13 +2124,13 @@
         <v>2021</v>
       </c>
       <c r="D82" s="5">
-        <v>45100</v>
+        <v>45200</v>
       </c>
       <c r="E82" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A83">
         <v>9014</v>
       </c>
@@ -2135,13 +2141,13 @@
         <v>2021</v>
       </c>
       <c r="D83" s="5">
-        <v>48900</v>
+        <v>49000</v>
       </c>
       <c r="E83" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A84">
         <v>9015</v>
       </c>
@@ -2152,13 +2158,13 @@
         <v>2021</v>
       </c>
       <c r="D84" s="5">
-        <v>45700</v>
+        <v>45800</v>
       </c>
       <c r="E84" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>110</v>
       </c>
@@ -2175,7 +2181,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A86">
         <v>9423</v>
       </c>
@@ -2186,13 +2192,13 @@
         <v>2021</v>
       </c>
       <c r="D86" s="5">
-        <v>50950</v>
+        <v>51050</v>
       </c>
       <c r="E86" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A87">
         <v>9427</v>
       </c>
@@ -2203,13 +2209,13 @@
         <v>2021</v>
       </c>
       <c r="D87" s="5">
-        <v>52350</v>
+        <v>52450</v>
       </c>
       <c r="E87" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A88">
         <v>9447</v>
       </c>
@@ -2220,13 +2226,13 @@
         <v>2021</v>
       </c>
       <c r="D88" s="5">
-        <v>53520</v>
+        <v>53620</v>
       </c>
       <c r="E88" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A89">
         <v>9432</v>
       </c>
@@ -2237,13 +2243,13 @@
         <v>2021</v>
       </c>
       <c r="D89" s="5">
-        <v>53900</v>
+        <v>54000</v>
       </c>
       <c r="E89" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A90">
         <v>9436</v>
       </c>
@@ -2254,13 +2260,13 @@
         <v>2021</v>
       </c>
       <c r="D90" s="5">
-        <v>55300</v>
+        <v>55400</v>
       </c>
       <c r="E90" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A91">
         <v>9457</v>
       </c>
@@ -2271,14 +2277,14 @@
         <v>2021</v>
       </c>
       <c r="D91" s="5">
-        <v>57110</v>
+        <v>57210</v>
       </c>
       <c r="E91" s="1">
         <v>1025</v>
       </c>
       <c r="J91" s="1"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>107</v>
       </c>
@@ -2289,14 +2295,14 @@
         <v>2021</v>
       </c>
       <c r="D92" s="5">
-        <v>49235</v>
+        <v>49335</v>
       </c>
       <c r="E92" s="1">
         <v>1025</v>
       </c>
       <c r="K92" s="1"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>108</v>
       </c>
@@ -2307,14 +2313,14 @@
         <v>2021</v>
       </c>
       <c r="D93" s="5">
-        <v>50635</v>
+        <v>50735</v>
       </c>
       <c r="E93" s="1">
         <v>1025</v>
       </c>
       <c r="K93" s="1"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
         <v>109</v>
       </c>
@@ -2325,14 +2331,14 @@
         <v>2021</v>
       </c>
       <c r="D94" s="5">
-        <v>51885</v>
+        <v>51985</v>
       </c>
       <c r="E94" s="1">
         <v>1025</v>
       </c>
       <c r="K94" s="1"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>112</v>
       </c>
@@ -2343,14 +2349,14 @@
         <v>2021</v>
       </c>
       <c r="D95" s="5">
-        <v>49160</v>
+        <v>48835</v>
       </c>
       <c r="E95" s="1">
         <v>1025</v>
       </c>
       <c r="K95" s="1"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>113</v>
       </c>
@@ -2361,13 +2367,13 @@
         <v>2021</v>
       </c>
       <c r="D96" s="5">
-        <v>51335</v>
+        <v>51010</v>
       </c>
       <c r="E96" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>114</v>
       </c>
@@ -2378,13 +2384,13 @@
         <v>2021</v>
       </c>
       <c r="D97" s="5">
-        <v>52090</v>
+        <v>51765</v>
       </c>
       <c r="E97" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>115</v>
       </c>
@@ -2395,13 +2401,13 @@
         <v>2021</v>
       </c>
       <c r="D98" s="5">
-        <v>53700</v>
+        <v>53230</v>
       </c>
       <c r="E98" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B99" t="s">
         <v>122</v>
       </c>
@@ -2412,6 +2418,23 @@
         <v>123</v>
       </c>
       <c r="E99" s="1">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A100" t="s">
+        <v>125</v>
+      </c>
+      <c r="B100" t="s">
+        <v>124</v>
+      </c>
+      <c r="C100">
+        <v>2021</v>
+      </c>
+      <c r="D100" s="2">
+        <v>110420</v>
+      </c>
+      <c r="E100" s="1">
         <v>1025</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated global variable for legacy global nav authentication
</commit_message>
<xml_diff>
--- a/Data Files/prodMSRPs.xlsx
+++ b/Data Files/prodMSRPs.xlsx
@@ -731,18 +731,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D97" sqref="D97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.3984375" customWidth="1"/>
     <col min="2" max="2" width="55" customWidth="1"/>
     <col min="4" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>84</v>
       </c>
@@ -759,7 +759,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>9202</v>
       </c>
@@ -770,13 +770,13 @@
         <v>2021</v>
       </c>
       <c r="D2" s="2">
-        <v>42120</v>
+        <v>42220</v>
       </c>
       <c r="E2" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>9203</v>
       </c>
@@ -787,13 +787,13 @@
         <v>2021</v>
       </c>
       <c r="D3" s="2">
-        <v>46590</v>
+        <v>46690</v>
       </c>
       <c r="E3" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>9206</v>
       </c>
@@ -804,13 +804,13 @@
         <v>2021</v>
       </c>
       <c r="D4" s="2">
-        <v>44810</v>
+        <v>44910</v>
       </c>
       <c r="E4" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>9207</v>
       </c>
@@ -821,13 +821,13 @@
         <v>2021</v>
       </c>
       <c r="D5" s="2">
-        <v>48765</v>
+        <v>48865</v>
       </c>
       <c r="E5" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>9212</v>
       </c>
@@ -838,13 +838,13 @@
         <v>2021</v>
       </c>
       <c r="D6" s="2">
-        <v>45050</v>
+        <v>45150</v>
       </c>
       <c r="E6" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>9213</v>
       </c>
@@ -855,13 +855,13 @@
         <v>2021</v>
       </c>
       <c r="D7" s="2">
-        <v>49520</v>
+        <v>49620</v>
       </c>
       <c r="E7" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>9216</v>
       </c>
@@ -872,13 +872,13 @@
         <v>2021</v>
       </c>
       <c r="D8" s="2">
-        <v>47215</v>
+        <v>47315</v>
       </c>
       <c r="E8" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>9217</v>
       </c>
@@ -889,13 +889,13 @@
         <v>2021</v>
       </c>
       <c r="D9" s="2">
-        <v>51130</v>
+        <v>51230</v>
       </c>
       <c r="E9" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>9000</v>
       </c>
@@ -906,13 +906,13 @@
         <v>2021</v>
       </c>
       <c r="D10" s="2">
-        <v>39900</v>
+        <v>40000</v>
       </c>
       <c r="E10" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>9002</v>
       </c>
@@ -923,13 +923,13 @@
         <v>2021</v>
       </c>
       <c r="D11" s="2">
-        <v>45100</v>
+        <v>45200</v>
       </c>
       <c r="E11" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>9004</v>
       </c>
@@ -940,13 +940,13 @@
         <v>2021</v>
       </c>
       <c r="D12" s="2">
-        <v>48900</v>
+        <v>49000</v>
       </c>
       <c r="E12" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>9040</v>
       </c>
@@ -957,13 +957,13 @@
         <v>2021</v>
       </c>
       <c r="D13" s="2">
-        <v>41810</v>
+        <v>41910</v>
       </c>
       <c r="E13" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>9042</v>
       </c>
@@ -974,13 +974,13 @@
         <v>2021</v>
       </c>
       <c r="D14" s="2">
-        <v>47010</v>
+        <v>47110</v>
       </c>
       <c r="E14" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>9044</v>
       </c>
@@ -991,13 +991,13 @@
         <v>2021</v>
       </c>
       <c r="D15" s="2">
-        <v>50810</v>
+        <v>50910</v>
       </c>
       <c r="E15" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>9005</v>
       </c>
@@ -1008,13 +1008,13 @@
         <v>2021</v>
       </c>
       <c r="D16" s="2">
-        <v>45700</v>
+        <v>45800</v>
       </c>
       <c r="E16" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>9502</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1048,7 +1048,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>9506</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1082,7 +1082,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>9510</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1116,7 +1116,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>9516</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1150,7 +1150,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1164,7 +1164,7 @@
         <v>45200</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1178,7 +1178,7 @@
         <v>47250</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -1192,7 +1192,7 @@
         <v>49415</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -1206,7 +1206,7 @@
         <v>50155</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>9700</v>
       </c>
@@ -1217,13 +1217,13 @@
         <v>2021</v>
       </c>
       <c r="D29" s="2">
-        <v>53100</v>
+        <v>53250</v>
       </c>
       <c r="E29" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -1234,13 +1234,13 @@
         <v>2021</v>
       </c>
       <c r="D30" s="2">
-        <v>56190</v>
+        <v>56340</v>
       </c>
       <c r="E30" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>9710</v>
       </c>
@@ -1251,13 +1251,13 @@
         <v>2021</v>
       </c>
       <c r="D31" s="2">
-        <v>64365</v>
+        <v>64515</v>
       </c>
       <c r="E31" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>9625</v>
       </c>
@@ -1268,13 +1268,13 @@
         <v>2020</v>
       </c>
       <c r="D32" s="2">
-        <v>86580</v>
+        <v>86730</v>
       </c>
       <c r="E32" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>9620</v>
       </c>
@@ -1285,13 +1285,13 @@
         <v>2020</v>
       </c>
       <c r="D33" s="2">
-        <v>91580</v>
+        <v>91730</v>
       </c>
       <c r="E33" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>9820</v>
       </c>
@@ -1319,13 +1319,13 @@
         <v>2021</v>
       </c>
       <c r="D35" s="2">
-        <v>37510</v>
+        <v>37610</v>
       </c>
       <c r="E35" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>9824</v>
       </c>
@@ -1336,13 +1336,13 @@
         <v>2021</v>
       </c>
       <c r="D36" s="2">
-        <v>38910</v>
+        <v>39010</v>
       </c>
       <c r="E36" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>9830</v>
       </c>
@@ -1353,13 +1353,13 @@
         <v>2021</v>
       </c>
       <c r="D37" s="2">
-        <v>39610</v>
+        <v>39710</v>
       </c>
       <c r="E37" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>9834</v>
       </c>
@@ -1370,13 +1370,13 @@
         <v>2021</v>
       </c>
       <c r="D38" s="2">
-        <v>41010</v>
+        <v>41110</v>
       </c>
       <c r="E38" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>9821</v>
       </c>
@@ -1387,13 +1387,13 @@
         <v>2021</v>
       </c>
       <c r="D39" s="2">
-        <v>43960</v>
+        <v>44060</v>
       </c>
       <c r="E39" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>9825</v>
       </c>
@@ -1404,13 +1404,13 @@
         <v>2021</v>
       </c>
       <c r="D40" s="2">
-        <v>45360</v>
+        <v>45460</v>
       </c>
       <c r="E40" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>9844</v>
       </c>
@@ -1421,13 +1421,13 @@
         <v>2021</v>
       </c>
       <c r="D41" s="2">
-        <v>40060</v>
+        <v>40160</v>
       </c>
       <c r="E41" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>9845</v>
       </c>
@@ -1438,13 +1438,13 @@
         <v>2021</v>
       </c>
       <c r="D42" s="2">
-        <v>46510</v>
+        <v>46610</v>
       </c>
       <c r="E42" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>9846</v>
       </c>
@@ -1455,13 +1455,13 @@
         <v>2021</v>
       </c>
       <c r="D43" s="2">
-        <v>46810</v>
+        <v>46910</v>
       </c>
       <c r="E43" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>48</v>
       </c>
@@ -1478,7 +1478,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A45">
         <v>9120</v>
       </c>
@@ -1495,7 +1495,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A46">
         <v>9126</v>
       </c>
@@ -1512,7 +1512,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A47">
         <v>9122</v>
       </c>
@@ -1529,7 +1529,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A48">
         <v>9128</v>
       </c>
@@ -1546,7 +1546,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A49">
         <v>9140</v>
       </c>
@@ -1563,7 +1563,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A50">
         <v>9146</v>
       </c>
@@ -1580,7 +1580,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>56</v>
       </c>
@@ -1597,7 +1597,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>56</v>
       </c>
@@ -1614,7 +1614,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A53">
         <v>9225</v>
       </c>
@@ -1625,13 +1625,13 @@
         <v>2021</v>
       </c>
       <c r="D53" s="2">
-        <v>65875</v>
+        <v>65975</v>
       </c>
       <c r="E53" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A54">
         <v>9226</v>
       </c>
@@ -1642,13 +1642,13 @@
         <v>2021</v>
       </c>
       <c r="D54" s="2">
-        <v>97100</v>
+        <v>97625</v>
       </c>
       <c r="E54" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A55">
         <v>9420</v>
       </c>
@@ -1659,13 +1659,13 @@
         <v>2021</v>
       </c>
       <c r="D55" s="2">
-        <v>45070</v>
+        <v>45170</v>
       </c>
       <c r="E55" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A56">
         <v>9424</v>
       </c>
@@ -1676,13 +1676,13 @@
         <v>2021</v>
       </c>
       <c r="D56" s="2">
-        <v>46470</v>
+        <v>46570</v>
       </c>
       <c r="E56" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A57">
         <v>9430</v>
       </c>
@@ -1693,13 +1693,13 @@
         <v>2021</v>
       </c>
       <c r="D57" s="2">
-        <v>47900</v>
+        <v>48000</v>
       </c>
       <c r="E57" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A58">
         <v>9434</v>
       </c>
@@ -1710,13 +1710,13 @@
         <v>2021</v>
       </c>
       <c r="D58" s="2">
-        <v>49300</v>
+        <v>49400</v>
       </c>
       <c r="E58" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A59">
         <v>9422</v>
       </c>
@@ -1727,13 +1727,13 @@
         <v>2021</v>
       </c>
       <c r="D59" s="2">
-        <v>48550</v>
+        <v>48650</v>
       </c>
       <c r="E59" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A60">
         <v>9426</v>
       </c>
@@ -1744,13 +1744,13 @@
         <v>2021</v>
       </c>
       <c r="D60" s="2">
-        <v>49950</v>
+        <v>50050</v>
       </c>
       <c r="E60" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A61">
         <v>9444</v>
       </c>
@@ -1761,13 +1761,13 @@
         <v>2021</v>
       </c>
       <c r="D61" s="2">
-        <v>47720</v>
+        <v>47820</v>
       </c>
       <c r="E61" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A62">
         <v>9454</v>
       </c>
@@ -1778,13 +1778,13 @@
         <v>2021</v>
       </c>
       <c r="D62" s="2">
-        <v>51110</v>
+        <v>51210</v>
       </c>
       <c r="E62" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A63">
         <v>9446</v>
       </c>
@@ -1795,13 +1795,13 @@
         <v>2021</v>
       </c>
       <c r="D63" s="2">
-        <v>51200</v>
+        <v>51300</v>
       </c>
       <c r="E63" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A64">
         <v>9301</v>
       </c>
@@ -1818,7 +1818,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A65">
         <v>9313</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A66">
         <v>9300</v>
       </c>
@@ -1852,7 +1852,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A67">
         <v>9306</v>
       </c>
@@ -1869,7 +1869,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A68">
         <v>9314</v>
       </c>
@@ -1886,7 +1886,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A69">
         <v>9316</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A70">
         <v>9260</v>
       </c>
@@ -1914,13 +1914,13 @@
         <v>2021</v>
       </c>
       <c r="D70" s="2">
-        <v>92950</v>
+        <v>93050</v>
       </c>
       <c r="E70" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A71">
         <v>9264</v>
       </c>
@@ -1931,13 +1931,13 @@
         <v>2021</v>
       </c>
       <c r="D71" s="2">
-        <v>97510</v>
+        <v>97610</v>
       </c>
       <c r="E71" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A72">
         <v>9262</v>
       </c>
@@ -1948,13 +1948,13 @@
         <v>2021</v>
       </c>
       <c r="D72" s="2">
-        <v>101000</v>
+        <v>101100</v>
       </c>
       <c r="E72" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A73">
         <v>9720</v>
       </c>
@@ -1971,7 +1971,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A74">
         <v>9724</v>
       </c>
@@ -1988,7 +1988,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A75">
         <v>9732</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A76">
         <v>9736</v>
       </c>
@@ -2022,7 +2022,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A77">
         <v>9722</v>
       </c>
@@ -2039,7 +2039,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A78">
         <v>9738</v>
       </c>
@@ -2056,7 +2056,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A79">
         <v>9335</v>
       </c>
@@ -2073,7 +2073,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>91</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A81">
         <v>9012</v>
       </c>
@@ -2101,13 +2101,13 @@
         <v>2021</v>
       </c>
       <c r="D81" s="5">
-        <v>39900</v>
+        <v>40000</v>
       </c>
       <c r="E81" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A82">
         <v>9013</v>
       </c>
@@ -2118,13 +2118,13 @@
         <v>2021</v>
       </c>
       <c r="D82" s="5">
-        <v>45100</v>
+        <v>45200</v>
       </c>
       <c r="E82" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A83">
         <v>9014</v>
       </c>
@@ -2135,13 +2135,13 @@
         <v>2021</v>
       </c>
       <c r="D83" s="5">
-        <v>48900</v>
+        <v>49000</v>
       </c>
       <c r="E83" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A84">
         <v>9015</v>
       </c>
@@ -2152,13 +2152,13 @@
         <v>2021</v>
       </c>
       <c r="D84" s="5">
-        <v>45700</v>
+        <v>45800</v>
       </c>
       <c r="E84" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>110</v>
       </c>
@@ -2175,7 +2175,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A86">
         <v>9423</v>
       </c>
@@ -2186,13 +2186,13 @@
         <v>2021</v>
       </c>
       <c r="D86" s="5">
-        <v>50950</v>
+        <v>51050</v>
       </c>
       <c r="E86" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A87">
         <v>9427</v>
       </c>
@@ -2203,13 +2203,13 @@
         <v>2021</v>
       </c>
       <c r="D87" s="5">
-        <v>52350</v>
+        <v>52450</v>
       </c>
       <c r="E87" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A88">
         <v>9447</v>
       </c>
@@ -2220,13 +2220,13 @@
         <v>2021</v>
       </c>
       <c r="D88" s="5">
-        <v>53520</v>
+        <v>53620</v>
       </c>
       <c r="E88" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A89">
         <v>9432</v>
       </c>
@@ -2237,13 +2237,13 @@
         <v>2021</v>
       </c>
       <c r="D89" s="5">
-        <v>53900</v>
+        <v>54000</v>
       </c>
       <c r="E89" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A90">
         <v>9436</v>
       </c>
@@ -2254,13 +2254,13 @@
         <v>2021</v>
       </c>
       <c r="D90" s="5">
-        <v>55300</v>
+        <v>55400</v>
       </c>
       <c r="E90" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A91">
         <v>9457</v>
       </c>
@@ -2271,14 +2271,14 @@
         <v>2021</v>
       </c>
       <c r="D91" s="5">
-        <v>57110</v>
+        <v>57210</v>
       </c>
       <c r="E91" s="1">
         <v>1025</v>
       </c>
       <c r="J91" s="1"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>107</v>
       </c>
@@ -2289,14 +2289,14 @@
         <v>2021</v>
       </c>
       <c r="D92" s="5">
-        <v>49235</v>
+        <v>49335</v>
       </c>
       <c r="E92" s="1">
         <v>1025</v>
       </c>
       <c r="K92" s="1"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>108</v>
       </c>
@@ -2307,14 +2307,14 @@
         <v>2021</v>
       </c>
       <c r="D93" s="5">
-        <v>50635</v>
+        <v>50735</v>
       </c>
       <c r="E93" s="1">
         <v>1025</v>
       </c>
       <c r="K93" s="1"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
         <v>109</v>
       </c>
@@ -2325,14 +2325,14 @@
         <v>2021</v>
       </c>
       <c r="D94" s="5">
-        <v>51885</v>
+        <v>51985</v>
       </c>
       <c r="E94" s="1">
         <v>1025</v>
       </c>
       <c r="K94" s="1"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>112</v>
       </c>
@@ -2343,14 +2343,14 @@
         <v>2021</v>
       </c>
       <c r="D95" s="5">
-        <v>49160</v>
+        <v>48835</v>
       </c>
       <c r="E95" s="1">
         <v>1025</v>
       </c>
       <c r="K95" s="1"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>113</v>
       </c>
@@ -2361,13 +2361,13 @@
         <v>2021</v>
       </c>
       <c r="D96" s="5">
-        <v>51335</v>
+        <v>51010</v>
       </c>
       <c r="E96" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>114</v>
       </c>
@@ -2378,13 +2378,13 @@
         <v>2021</v>
       </c>
       <c r="D97" s="5">
-        <v>52090</v>
+        <v>51765</v>
       </c>
       <c r="E97" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>115</v>
       </c>
@@ -2395,13 +2395,13 @@
         <v>2021</v>
       </c>
       <c r="D98" s="5">
-        <v>53700</v>
+        <v>53230</v>
       </c>
       <c r="E98" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B99" t="s">
         <v>122</v>
       </c>

</xml_diff>

<commit_message>
offers query parameter test added
</commit_message>
<xml_diff>
--- a/Data Files/prodMSRPs.xlsx
+++ b/Data Files/prodMSRPs.xlsx
@@ -731,18 +731,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D99" sqref="D99"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D97" sqref="D97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.3984375" customWidth="1"/>
     <col min="2" max="2" width="55" customWidth="1"/>
     <col min="4" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>84</v>
       </c>
@@ -759,7 +759,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>9202</v>
       </c>
@@ -770,13 +770,13 @@
         <v>2021</v>
       </c>
       <c r="D2" s="2">
-        <v>42120</v>
+        <v>42220</v>
       </c>
       <c r="E2" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>9203</v>
       </c>
@@ -787,13 +787,13 @@
         <v>2021</v>
       </c>
       <c r="D3" s="2">
-        <v>46590</v>
+        <v>46690</v>
       </c>
       <c r="E3" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>9206</v>
       </c>
@@ -804,13 +804,13 @@
         <v>2021</v>
       </c>
       <c r="D4" s="2">
-        <v>44810</v>
+        <v>44910</v>
       </c>
       <c r="E4" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>9207</v>
       </c>
@@ -821,13 +821,13 @@
         <v>2021</v>
       </c>
       <c r="D5" s="2">
-        <v>48765</v>
+        <v>48865</v>
       </c>
       <c r="E5" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>9212</v>
       </c>
@@ -838,13 +838,13 @@
         <v>2021</v>
       </c>
       <c r="D6" s="2">
-        <v>45050</v>
+        <v>45150</v>
       </c>
       <c r="E6" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>9213</v>
       </c>
@@ -855,13 +855,13 @@
         <v>2021</v>
       </c>
       <c r="D7" s="2">
-        <v>49520</v>
+        <v>49620</v>
       </c>
       <c r="E7" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>9216</v>
       </c>
@@ -872,13 +872,13 @@
         <v>2021</v>
       </c>
       <c r="D8" s="2">
-        <v>47215</v>
+        <v>47315</v>
       </c>
       <c r="E8" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>9217</v>
       </c>
@@ -889,13 +889,13 @@
         <v>2021</v>
       </c>
       <c r="D9" s="2">
-        <v>51130</v>
+        <v>51230</v>
       </c>
       <c r="E9" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>9000</v>
       </c>
@@ -906,13 +906,13 @@
         <v>2021</v>
       </c>
       <c r="D10" s="2">
-        <v>39900</v>
+        <v>40000</v>
       </c>
       <c r="E10" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>9002</v>
       </c>
@@ -923,13 +923,13 @@
         <v>2021</v>
       </c>
       <c r="D11" s="2">
-        <v>45100</v>
+        <v>45200</v>
       </c>
       <c r="E11" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>9004</v>
       </c>
@@ -940,13 +940,13 @@
         <v>2021</v>
       </c>
       <c r="D12" s="2">
-        <v>48900</v>
+        <v>49000</v>
       </c>
       <c r="E12" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>9040</v>
       </c>
@@ -957,13 +957,13 @@
         <v>2021</v>
       </c>
       <c r="D13" s="2">
-        <v>41810</v>
+        <v>41910</v>
       </c>
       <c r="E13" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>9042</v>
       </c>
@@ -974,13 +974,13 @@
         <v>2021</v>
       </c>
       <c r="D14" s="2">
-        <v>47010</v>
+        <v>47110</v>
       </c>
       <c r="E14" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>9044</v>
       </c>
@@ -991,13 +991,13 @@
         <v>2021</v>
       </c>
       <c r="D15" s="2">
-        <v>50810</v>
+        <v>50910</v>
       </c>
       <c r="E15" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>9005</v>
       </c>
@@ -1008,13 +1008,13 @@
         <v>2021</v>
       </c>
       <c r="D16" s="2">
-        <v>45700</v>
+        <v>45800</v>
       </c>
       <c r="E16" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>9502</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1048,7 +1048,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>9506</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1082,7 +1082,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>9510</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1116,7 +1116,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>9516</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1150,7 +1150,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1164,7 +1164,7 @@
         <v>45200</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1178,7 +1178,7 @@
         <v>47250</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -1192,7 +1192,7 @@
         <v>49415</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -1206,7 +1206,7 @@
         <v>50155</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>9700</v>
       </c>
@@ -1214,16 +1214,16 @@
         <v>32</v>
       </c>
       <c r="C29">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D29" s="2">
-        <v>53100</v>
+        <v>53250</v>
       </c>
       <c r="E29" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -1231,16 +1231,16 @@
         <v>34</v>
       </c>
       <c r="C30">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D30" s="2">
-        <v>55890</v>
+        <v>56340</v>
       </c>
       <c r="E30" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>9710</v>
       </c>
@@ -1248,16 +1248,16 @@
         <v>35</v>
       </c>
       <c r="C31">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D31" s="2">
-        <v>64365</v>
+        <v>64515</v>
       </c>
       <c r="E31" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>9625</v>
       </c>
@@ -1268,13 +1268,13 @@
         <v>2020</v>
       </c>
       <c r="D32" s="2">
-        <v>86580</v>
+        <v>86730</v>
       </c>
       <c r="E32" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>9620</v>
       </c>
@@ -1285,13 +1285,13 @@
         <v>2020</v>
       </c>
       <c r="D33" s="2">
-        <v>91580</v>
+        <v>91730</v>
       </c>
       <c r="E33" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>9820</v>
       </c>
@@ -1319,13 +1319,13 @@
         <v>2021</v>
       </c>
       <c r="D35" s="2">
-        <v>37510</v>
+        <v>37610</v>
       </c>
       <c r="E35" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>9824</v>
       </c>
@@ -1336,13 +1336,13 @@
         <v>2021</v>
       </c>
       <c r="D36" s="2">
-        <v>38910</v>
+        <v>39010</v>
       </c>
       <c r="E36" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>9830</v>
       </c>
@@ -1353,13 +1353,13 @@
         <v>2021</v>
       </c>
       <c r="D37" s="2">
-        <v>39610</v>
+        <v>39710</v>
       </c>
       <c r="E37" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>9834</v>
       </c>
@@ -1370,13 +1370,13 @@
         <v>2021</v>
       </c>
       <c r="D38" s="2">
-        <v>41010</v>
+        <v>41110</v>
       </c>
       <c r="E38" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>9821</v>
       </c>
@@ -1387,13 +1387,13 @@
         <v>2021</v>
       </c>
       <c r="D39" s="2">
-        <v>43960</v>
+        <v>44060</v>
       </c>
       <c r="E39" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>9825</v>
       </c>
@@ -1404,13 +1404,13 @@
         <v>2021</v>
       </c>
       <c r="D40" s="2">
-        <v>45360</v>
+        <v>45460</v>
       </c>
       <c r="E40" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>9844</v>
       </c>
@@ -1421,13 +1421,13 @@
         <v>2021</v>
       </c>
       <c r="D41" s="2">
-        <v>40060</v>
+        <v>40160</v>
       </c>
       <c r="E41" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>9845</v>
       </c>
@@ -1438,13 +1438,13 @@
         <v>2021</v>
       </c>
       <c r="D42" s="2">
-        <v>46510</v>
+        <v>46610</v>
       </c>
       <c r="E42" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>9846</v>
       </c>
@@ -1455,13 +1455,13 @@
         <v>2021</v>
       </c>
       <c r="D43" s="2">
-        <v>46810</v>
+        <v>46910</v>
       </c>
       <c r="E43" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>48</v>
       </c>
@@ -1478,7 +1478,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A45">
         <v>9120</v>
       </c>
@@ -1486,16 +1486,16 @@
         <v>50</v>
       </c>
       <c r="C45">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D45" s="2">
-        <v>75450</v>
+        <v>76000</v>
       </c>
       <c r="E45" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A46">
         <v>9126</v>
       </c>
@@ -1503,16 +1503,16 @@
         <v>51</v>
       </c>
       <c r="C46">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D46" s="2">
-        <v>78670</v>
+        <v>79250</v>
       </c>
       <c r="E46" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A47">
         <v>9122</v>
       </c>
@@ -1520,16 +1520,16 @@
         <v>52</v>
       </c>
       <c r="C47">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D47" s="2">
-        <v>81450</v>
+        <v>79600</v>
       </c>
       <c r="E47" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A48">
         <v>9128</v>
       </c>
@@ -1537,16 +1537,16 @@
         <v>53</v>
       </c>
       <c r="C48">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D48" s="2">
-        <v>84670</v>
+        <v>82850</v>
       </c>
       <c r="E48" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A49">
         <v>9140</v>
       </c>
@@ -1563,7 +1563,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A50">
         <v>9146</v>
       </c>
@@ -1580,7 +1580,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>56</v>
       </c>
@@ -1597,7 +1597,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>56</v>
       </c>
@@ -1614,7 +1614,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A53">
         <v>9225</v>
       </c>
@@ -1625,13 +1625,13 @@
         <v>2021</v>
       </c>
       <c r="D53" s="2">
-        <v>65875</v>
+        <v>65975</v>
       </c>
       <c r="E53" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A54">
         <v>9226</v>
       </c>
@@ -1642,13 +1642,13 @@
         <v>2021</v>
       </c>
       <c r="D54" s="2">
-        <v>97100</v>
+        <v>97625</v>
       </c>
       <c r="E54" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A55">
         <v>9420</v>
       </c>
@@ -1659,13 +1659,13 @@
         <v>2021</v>
       </c>
       <c r="D55" s="2">
-        <v>45070</v>
+        <v>45170</v>
       </c>
       <c r="E55" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A56">
         <v>9424</v>
       </c>
@@ -1676,13 +1676,13 @@
         <v>2021</v>
       </c>
       <c r="D56" s="2">
-        <v>46470</v>
+        <v>46570</v>
       </c>
       <c r="E56" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A57">
         <v>9430</v>
       </c>
@@ -1693,13 +1693,13 @@
         <v>2021</v>
       </c>
       <c r="D57" s="2">
-        <v>47900</v>
+        <v>48000</v>
       </c>
       <c r="E57" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A58">
         <v>9434</v>
       </c>
@@ -1710,13 +1710,13 @@
         <v>2021</v>
       </c>
       <c r="D58" s="2">
-        <v>49300</v>
+        <v>49400</v>
       </c>
       <c r="E58" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A59">
         <v>9422</v>
       </c>
@@ -1727,13 +1727,13 @@
         <v>2021</v>
       </c>
       <c r="D59" s="2">
-        <v>48550</v>
+        <v>48650</v>
       </c>
       <c r="E59" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A60">
         <v>9426</v>
       </c>
@@ -1744,13 +1744,13 @@
         <v>2021</v>
       </c>
       <c r="D60" s="2">
-        <v>49950</v>
+        <v>50050</v>
       </c>
       <c r="E60" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A61">
         <v>9444</v>
       </c>
@@ -1761,13 +1761,13 @@
         <v>2021</v>
       </c>
       <c r="D61" s="2">
-        <v>47720</v>
+        <v>47820</v>
       </c>
       <c r="E61" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A62">
         <v>9454</v>
       </c>
@@ -1778,13 +1778,13 @@
         <v>2021</v>
       </c>
       <c r="D62" s="2">
-        <v>51110</v>
+        <v>51210</v>
       </c>
       <c r="E62" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A63">
         <v>9446</v>
       </c>
@@ -1795,13 +1795,13 @@
         <v>2021</v>
       </c>
       <c r="D63" s="2">
-        <v>51200</v>
+        <v>51300</v>
       </c>
       <c r="E63" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A64">
         <v>9301</v>
       </c>
@@ -1818,7 +1818,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A65">
         <v>9313</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A66">
         <v>9300</v>
       </c>
@@ -1852,7 +1852,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A67">
         <v>9306</v>
       </c>
@@ -1869,7 +1869,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A68">
         <v>9314</v>
       </c>
@@ -1886,7 +1886,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A69">
         <v>9316</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A70">
         <v>9260</v>
       </c>
@@ -1914,13 +1914,13 @@
         <v>2021</v>
       </c>
       <c r="D70" s="2">
-        <v>92950</v>
+        <v>93050</v>
       </c>
       <c r="E70" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A71">
         <v>9264</v>
       </c>
@@ -1931,13 +1931,13 @@
         <v>2021</v>
       </c>
       <c r="D71" s="2">
-        <v>97510</v>
+        <v>97610</v>
       </c>
       <c r="E71" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A72">
         <v>9262</v>
       </c>
@@ -1948,13 +1948,13 @@
         <v>2021</v>
       </c>
       <c r="D72" s="2">
-        <v>101000</v>
+        <v>101100</v>
       </c>
       <c r="E72" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A73">
         <v>9720</v>
       </c>
@@ -1971,7 +1971,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A74">
         <v>9724</v>
       </c>
@@ -1988,7 +1988,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A75">
         <v>9732</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A76">
         <v>9736</v>
       </c>
@@ -2022,7 +2022,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A77">
         <v>9722</v>
       </c>
@@ -2039,7 +2039,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A78">
         <v>9738</v>
       </c>
@@ -2056,7 +2056,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A79">
         <v>9335</v>
       </c>
@@ -2073,7 +2073,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>91</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A81">
         <v>9012</v>
       </c>
@@ -2101,13 +2101,13 @@
         <v>2021</v>
       </c>
       <c r="D81" s="5">
-        <v>39900</v>
+        <v>40000</v>
       </c>
       <c r="E81" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A82">
         <v>9013</v>
       </c>
@@ -2118,13 +2118,13 @@
         <v>2021</v>
       </c>
       <c r="D82" s="5">
-        <v>45100</v>
+        <v>45200</v>
       </c>
       <c r="E82" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A83">
         <v>9014</v>
       </c>
@@ -2135,13 +2135,13 @@
         <v>2021</v>
       </c>
       <c r="D83" s="5">
-        <v>48900</v>
+        <v>49000</v>
       </c>
       <c r="E83" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A84">
         <v>9015</v>
       </c>
@@ -2152,13 +2152,13 @@
         <v>2021</v>
       </c>
       <c r="D84" s="5">
-        <v>45700</v>
+        <v>45800</v>
       </c>
       <c r="E84" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>110</v>
       </c>
@@ -2175,7 +2175,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A86">
         <v>9423</v>
       </c>
@@ -2186,13 +2186,13 @@
         <v>2021</v>
       </c>
       <c r="D86" s="5">
-        <v>50950</v>
+        <v>51050</v>
       </c>
       <c r="E86" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A87">
         <v>9427</v>
       </c>
@@ -2203,13 +2203,13 @@
         <v>2021</v>
       </c>
       <c r="D87" s="5">
-        <v>52350</v>
+        <v>52450</v>
       </c>
       <c r="E87" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A88">
         <v>9447</v>
       </c>
@@ -2220,13 +2220,13 @@
         <v>2021</v>
       </c>
       <c r="D88" s="5">
-        <v>53520</v>
+        <v>53620</v>
       </c>
       <c r="E88" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A89">
         <v>9432</v>
       </c>
@@ -2237,13 +2237,13 @@
         <v>2021</v>
       </c>
       <c r="D89" s="5">
-        <v>53900</v>
+        <v>54000</v>
       </c>
       <c r="E89" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A90">
         <v>9436</v>
       </c>
@@ -2254,13 +2254,13 @@
         <v>2021</v>
       </c>
       <c r="D90" s="5">
-        <v>55300</v>
+        <v>55400</v>
       </c>
       <c r="E90" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A91">
         <v>9457</v>
       </c>
@@ -2271,14 +2271,14 @@
         <v>2021</v>
       </c>
       <c r="D91" s="5">
-        <v>57110</v>
+        <v>57210</v>
       </c>
       <c r="E91" s="1">
         <v>1025</v>
       </c>
       <c r="J91" s="1"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>107</v>
       </c>
@@ -2289,14 +2289,14 @@
         <v>2021</v>
       </c>
       <c r="D92" s="5">
-        <v>49235</v>
+        <v>49335</v>
       </c>
       <c r="E92" s="1">
         <v>1025</v>
       </c>
       <c r="K92" s="1"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>108</v>
       </c>
@@ -2307,14 +2307,14 @@
         <v>2021</v>
       </c>
       <c r="D93" s="5">
-        <v>50635</v>
+        <v>50735</v>
       </c>
       <c r="E93" s="1">
         <v>1025</v>
       </c>
       <c r="K93" s="1"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
         <v>109</v>
       </c>
@@ -2325,14 +2325,14 @@
         <v>2021</v>
       </c>
       <c r="D94" s="5">
-        <v>51885</v>
+        <v>51985</v>
       </c>
       <c r="E94" s="1">
         <v>1025</v>
       </c>
       <c r="K94" s="1"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>112</v>
       </c>
@@ -2343,14 +2343,14 @@
         <v>2021</v>
       </c>
       <c r="D95" s="5">
-        <v>49160</v>
+        <v>48835</v>
       </c>
       <c r="E95" s="1">
         <v>1025</v>
       </c>
       <c r="K95" s="1"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>113</v>
       </c>
@@ -2361,13 +2361,13 @@
         <v>2021</v>
       </c>
       <c r="D96" s="5">
-        <v>51335</v>
+        <v>51010</v>
       </c>
       <c r="E96" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>114</v>
       </c>
@@ -2378,13 +2378,13 @@
         <v>2021</v>
       </c>
       <c r="D97" s="5">
-        <v>52090</v>
+        <v>51765</v>
       </c>
       <c r="E97" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>115</v>
       </c>
@@ -2395,13 +2395,13 @@
         <v>2021</v>
       </c>
       <c r="D98" s="5">
-        <v>53700</v>
+        <v>53230</v>
       </c>
       <c r="E98" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B99" t="s">
         <v>122</v>
       </c>

</xml_diff>

<commit_message>
updated service down test zip to 00003
</commit_message>
<xml_diff>
--- a/Data Files/prodMSRPs.xlsx
+++ b/Data Files/prodMSRPs.xlsx
@@ -731,18 +731,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D99" sqref="D99"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D97" sqref="D97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.3984375" customWidth="1"/>
     <col min="2" max="2" width="55" customWidth="1"/>
     <col min="4" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>84</v>
       </c>
@@ -759,7 +759,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>9202</v>
       </c>
@@ -770,13 +770,13 @@
         <v>2021</v>
       </c>
       <c r="D2" s="2">
-        <v>42120</v>
+        <v>42220</v>
       </c>
       <c r="E2" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>9203</v>
       </c>
@@ -787,13 +787,13 @@
         <v>2021</v>
       </c>
       <c r="D3" s="2">
-        <v>46590</v>
+        <v>46690</v>
       </c>
       <c r="E3" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>9206</v>
       </c>
@@ -804,13 +804,13 @@
         <v>2021</v>
       </c>
       <c r="D4" s="2">
-        <v>44810</v>
+        <v>44910</v>
       </c>
       <c r="E4" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>9207</v>
       </c>
@@ -821,13 +821,13 @@
         <v>2021</v>
       </c>
       <c r="D5" s="2">
-        <v>48765</v>
+        <v>48865</v>
       </c>
       <c r="E5" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>9212</v>
       </c>
@@ -838,13 +838,13 @@
         <v>2021</v>
       </c>
       <c r="D6" s="2">
-        <v>45050</v>
+        <v>45150</v>
       </c>
       <c r="E6" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>9213</v>
       </c>
@@ -855,13 +855,13 @@
         <v>2021</v>
       </c>
       <c r="D7" s="2">
-        <v>49520</v>
+        <v>49620</v>
       </c>
       <c r="E7" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>9216</v>
       </c>
@@ -872,13 +872,13 @@
         <v>2021</v>
       </c>
       <c r="D8" s="2">
-        <v>47215</v>
+        <v>47315</v>
       </c>
       <c r="E8" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>9217</v>
       </c>
@@ -889,13 +889,13 @@
         <v>2021</v>
       </c>
       <c r="D9" s="2">
-        <v>51130</v>
+        <v>51230</v>
       </c>
       <c r="E9" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>9000</v>
       </c>
@@ -906,13 +906,13 @@
         <v>2021</v>
       </c>
       <c r="D10" s="2">
-        <v>39900</v>
+        <v>40000</v>
       </c>
       <c r="E10" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>9002</v>
       </c>
@@ -923,13 +923,13 @@
         <v>2021</v>
       </c>
       <c r="D11" s="2">
-        <v>45100</v>
+        <v>45200</v>
       </c>
       <c r="E11" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>9004</v>
       </c>
@@ -940,13 +940,13 @@
         <v>2021</v>
       </c>
       <c r="D12" s="2">
-        <v>48900</v>
+        <v>49000</v>
       </c>
       <c r="E12" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>9040</v>
       </c>
@@ -957,13 +957,13 @@
         <v>2021</v>
       </c>
       <c r="D13" s="2">
-        <v>41810</v>
+        <v>41910</v>
       </c>
       <c r="E13" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>9042</v>
       </c>
@@ -974,13 +974,13 @@
         <v>2021</v>
       </c>
       <c r="D14" s="2">
-        <v>47010</v>
+        <v>47110</v>
       </c>
       <c r="E14" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>9044</v>
       </c>
@@ -991,13 +991,13 @@
         <v>2021</v>
       </c>
       <c r="D15" s="2">
-        <v>50810</v>
+        <v>50910</v>
       </c>
       <c r="E15" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>9005</v>
       </c>
@@ -1008,13 +1008,13 @@
         <v>2021</v>
       </c>
       <c r="D16" s="2">
-        <v>45700</v>
+        <v>45800</v>
       </c>
       <c r="E16" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>9502</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1048,7 +1048,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>9506</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1082,7 +1082,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>9510</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1116,7 +1116,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>9516</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1150,7 +1150,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1164,7 +1164,7 @@
         <v>45200</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1178,7 +1178,7 @@
         <v>47250</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -1192,7 +1192,7 @@
         <v>49415</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -1206,7 +1206,7 @@
         <v>50155</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>9700</v>
       </c>
@@ -1214,16 +1214,16 @@
         <v>32</v>
       </c>
       <c r="C29">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D29" s="2">
-        <v>53100</v>
+        <v>53250</v>
       </c>
       <c r="E29" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -1231,16 +1231,16 @@
         <v>34</v>
       </c>
       <c r="C30">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D30" s="2">
-        <v>55890</v>
+        <v>56340</v>
       </c>
       <c r="E30" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>9710</v>
       </c>
@@ -1248,16 +1248,16 @@
         <v>35</v>
       </c>
       <c r="C31">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D31" s="2">
-        <v>64365</v>
+        <v>64515</v>
       </c>
       <c r="E31" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>9625</v>
       </c>
@@ -1268,13 +1268,13 @@
         <v>2020</v>
       </c>
       <c r="D32" s="2">
-        <v>86580</v>
+        <v>86730</v>
       </c>
       <c r="E32" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>9620</v>
       </c>
@@ -1285,13 +1285,13 @@
         <v>2020</v>
       </c>
       <c r="D33" s="2">
-        <v>91580</v>
+        <v>91730</v>
       </c>
       <c r="E33" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>9820</v>
       </c>
@@ -1319,13 +1319,13 @@
         <v>2021</v>
       </c>
       <c r="D35" s="2">
-        <v>37510</v>
+        <v>37610</v>
       </c>
       <c r="E35" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>9824</v>
       </c>
@@ -1336,13 +1336,13 @@
         <v>2021</v>
       </c>
       <c r="D36" s="2">
-        <v>38910</v>
+        <v>39010</v>
       </c>
       <c r="E36" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>9830</v>
       </c>
@@ -1353,13 +1353,13 @@
         <v>2021</v>
       </c>
       <c r="D37" s="2">
-        <v>39610</v>
+        <v>39710</v>
       </c>
       <c r="E37" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>9834</v>
       </c>
@@ -1370,13 +1370,13 @@
         <v>2021</v>
       </c>
       <c r="D38" s="2">
-        <v>41010</v>
+        <v>41110</v>
       </c>
       <c r="E38" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>9821</v>
       </c>
@@ -1387,13 +1387,13 @@
         <v>2021</v>
       </c>
       <c r="D39" s="2">
-        <v>43960</v>
+        <v>44060</v>
       </c>
       <c r="E39" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>9825</v>
       </c>
@@ -1404,13 +1404,13 @@
         <v>2021</v>
       </c>
       <c r="D40" s="2">
-        <v>45360</v>
+        <v>45460</v>
       </c>
       <c r="E40" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>9844</v>
       </c>
@@ -1421,13 +1421,13 @@
         <v>2021</v>
       </c>
       <c r="D41" s="2">
-        <v>40060</v>
+        <v>40160</v>
       </c>
       <c r="E41" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>9845</v>
       </c>
@@ -1438,13 +1438,13 @@
         <v>2021</v>
       </c>
       <c r="D42" s="2">
-        <v>46510</v>
+        <v>46610</v>
       </c>
       <c r="E42" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>9846</v>
       </c>
@@ -1455,13 +1455,13 @@
         <v>2021</v>
       </c>
       <c r="D43" s="2">
-        <v>46810</v>
+        <v>46910</v>
       </c>
       <c r="E43" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>48</v>
       </c>
@@ -1478,7 +1478,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A45">
         <v>9120</v>
       </c>
@@ -1486,16 +1486,16 @@
         <v>50</v>
       </c>
       <c r="C45">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D45" s="2">
-        <v>75450</v>
+        <v>76000</v>
       </c>
       <c r="E45" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A46">
         <v>9126</v>
       </c>
@@ -1503,16 +1503,16 @@
         <v>51</v>
       </c>
       <c r="C46">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D46" s="2">
-        <v>78670</v>
+        <v>79250</v>
       </c>
       <c r="E46" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A47">
         <v>9122</v>
       </c>
@@ -1520,16 +1520,16 @@
         <v>52</v>
       </c>
       <c r="C47">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D47" s="2">
-        <v>81450</v>
+        <v>79600</v>
       </c>
       <c r="E47" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A48">
         <v>9128</v>
       </c>
@@ -1537,16 +1537,16 @@
         <v>53</v>
       </c>
       <c r="C48">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D48" s="2">
-        <v>84670</v>
+        <v>82850</v>
       </c>
       <c r="E48" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A49">
         <v>9140</v>
       </c>
@@ -1563,7 +1563,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A50">
         <v>9146</v>
       </c>
@@ -1580,7 +1580,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>56</v>
       </c>
@@ -1597,7 +1597,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>56</v>
       </c>
@@ -1614,7 +1614,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A53">
         <v>9225</v>
       </c>
@@ -1625,13 +1625,13 @@
         <v>2021</v>
       </c>
       <c r="D53" s="2">
-        <v>65875</v>
+        <v>65975</v>
       </c>
       <c r="E53" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A54">
         <v>9226</v>
       </c>
@@ -1642,13 +1642,13 @@
         <v>2021</v>
       </c>
       <c r="D54" s="2">
-        <v>97100</v>
+        <v>97625</v>
       </c>
       <c r="E54" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A55">
         <v>9420</v>
       </c>
@@ -1659,13 +1659,13 @@
         <v>2021</v>
       </c>
       <c r="D55" s="2">
-        <v>45070</v>
+        <v>45170</v>
       </c>
       <c r="E55" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A56">
         <v>9424</v>
       </c>
@@ -1676,13 +1676,13 @@
         <v>2021</v>
       </c>
       <c r="D56" s="2">
-        <v>46470</v>
+        <v>46570</v>
       </c>
       <c r="E56" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A57">
         <v>9430</v>
       </c>
@@ -1693,13 +1693,13 @@
         <v>2021</v>
       </c>
       <c r="D57" s="2">
-        <v>47900</v>
+        <v>48000</v>
       </c>
       <c r="E57" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A58">
         <v>9434</v>
       </c>
@@ -1710,13 +1710,13 @@
         <v>2021</v>
       </c>
       <c r="D58" s="2">
-        <v>49300</v>
+        <v>49400</v>
       </c>
       <c r="E58" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A59">
         <v>9422</v>
       </c>
@@ -1727,13 +1727,13 @@
         <v>2021</v>
       </c>
       <c r="D59" s="2">
-        <v>48550</v>
+        <v>48650</v>
       </c>
       <c r="E59" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A60">
         <v>9426</v>
       </c>
@@ -1744,13 +1744,13 @@
         <v>2021</v>
       </c>
       <c r="D60" s="2">
-        <v>49950</v>
+        <v>50050</v>
       </c>
       <c r="E60" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A61">
         <v>9444</v>
       </c>
@@ -1761,13 +1761,13 @@
         <v>2021</v>
       </c>
       <c r="D61" s="2">
-        <v>47720</v>
+        <v>47820</v>
       </c>
       <c r="E61" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A62">
         <v>9454</v>
       </c>
@@ -1778,13 +1778,13 @@
         <v>2021</v>
       </c>
       <c r="D62" s="2">
-        <v>51110</v>
+        <v>51210</v>
       </c>
       <c r="E62" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A63">
         <v>9446</v>
       </c>
@@ -1795,13 +1795,13 @@
         <v>2021</v>
       </c>
       <c r="D63" s="2">
-        <v>51200</v>
+        <v>51300</v>
       </c>
       <c r="E63" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A64">
         <v>9301</v>
       </c>
@@ -1818,7 +1818,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A65">
         <v>9313</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A66">
         <v>9300</v>
       </c>
@@ -1852,7 +1852,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A67">
         <v>9306</v>
       </c>
@@ -1869,7 +1869,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A68">
         <v>9314</v>
       </c>
@@ -1886,7 +1886,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A69">
         <v>9316</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A70">
         <v>9260</v>
       </c>
@@ -1914,13 +1914,13 @@
         <v>2021</v>
       </c>
       <c r="D70" s="2">
-        <v>92950</v>
+        <v>93050</v>
       </c>
       <c r="E70" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A71">
         <v>9264</v>
       </c>
@@ -1931,13 +1931,13 @@
         <v>2021</v>
       </c>
       <c r="D71" s="2">
-        <v>97510</v>
+        <v>97610</v>
       </c>
       <c r="E71" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A72">
         <v>9262</v>
       </c>
@@ -1948,13 +1948,13 @@
         <v>2021</v>
       </c>
       <c r="D72" s="2">
-        <v>101000</v>
+        <v>101100</v>
       </c>
       <c r="E72" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A73">
         <v>9720</v>
       </c>
@@ -1971,7 +1971,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A74">
         <v>9724</v>
       </c>
@@ -1988,7 +1988,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A75">
         <v>9732</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A76">
         <v>9736</v>
       </c>
@@ -2022,7 +2022,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A77">
         <v>9722</v>
       </c>
@@ -2039,7 +2039,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A78">
         <v>9738</v>
       </c>
@@ -2056,7 +2056,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A79">
         <v>9335</v>
       </c>
@@ -2073,7 +2073,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>91</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A81">
         <v>9012</v>
       </c>
@@ -2101,13 +2101,13 @@
         <v>2021</v>
       </c>
       <c r="D81" s="5">
-        <v>39900</v>
+        <v>40000</v>
       </c>
       <c r="E81" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A82">
         <v>9013</v>
       </c>
@@ -2118,13 +2118,13 @@
         <v>2021</v>
       </c>
       <c r="D82" s="5">
-        <v>45100</v>
+        <v>45200</v>
       </c>
       <c r="E82" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A83">
         <v>9014</v>
       </c>
@@ -2135,13 +2135,13 @@
         <v>2021</v>
       </c>
       <c r="D83" s="5">
-        <v>48900</v>
+        <v>49000</v>
       </c>
       <c r="E83" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A84">
         <v>9015</v>
       </c>
@@ -2152,13 +2152,13 @@
         <v>2021</v>
       </c>
       <c r="D84" s="5">
-        <v>45700</v>
+        <v>45800</v>
       </c>
       <c r="E84" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>110</v>
       </c>
@@ -2175,7 +2175,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A86">
         <v>9423</v>
       </c>
@@ -2186,13 +2186,13 @@
         <v>2021</v>
       </c>
       <c r="D86" s="5">
-        <v>50950</v>
+        <v>51050</v>
       </c>
       <c r="E86" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A87">
         <v>9427</v>
       </c>
@@ -2203,13 +2203,13 @@
         <v>2021</v>
       </c>
       <c r="D87" s="5">
-        <v>52350</v>
+        <v>52450</v>
       </c>
       <c r="E87" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A88">
         <v>9447</v>
       </c>
@@ -2220,13 +2220,13 @@
         <v>2021</v>
       </c>
       <c r="D88" s="5">
-        <v>53520</v>
+        <v>53620</v>
       </c>
       <c r="E88" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A89">
         <v>9432</v>
       </c>
@@ -2237,13 +2237,13 @@
         <v>2021</v>
       </c>
       <c r="D89" s="5">
-        <v>53900</v>
+        <v>54000</v>
       </c>
       <c r="E89" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A90">
         <v>9436</v>
       </c>
@@ -2254,13 +2254,13 @@
         <v>2021</v>
       </c>
       <c r="D90" s="5">
-        <v>55300</v>
+        <v>55400</v>
       </c>
       <c r="E90" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A91">
         <v>9457</v>
       </c>
@@ -2271,14 +2271,14 @@
         <v>2021</v>
       </c>
       <c r="D91" s="5">
-        <v>57110</v>
+        <v>57210</v>
       </c>
       <c r="E91" s="1">
         <v>1025</v>
       </c>
       <c r="J91" s="1"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>107</v>
       </c>
@@ -2289,14 +2289,14 @@
         <v>2021</v>
       </c>
       <c r="D92" s="5">
-        <v>49235</v>
+        <v>49335</v>
       </c>
       <c r="E92" s="1">
         <v>1025</v>
       </c>
       <c r="K92" s="1"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>108</v>
       </c>
@@ -2307,14 +2307,14 @@
         <v>2021</v>
       </c>
       <c r="D93" s="5">
-        <v>50635</v>
+        <v>50735</v>
       </c>
       <c r="E93" s="1">
         <v>1025</v>
       </c>
       <c r="K93" s="1"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
         <v>109</v>
       </c>
@@ -2325,14 +2325,14 @@
         <v>2021</v>
       </c>
       <c r="D94" s="5">
-        <v>51885</v>
+        <v>51985</v>
       </c>
       <c r="E94" s="1">
         <v>1025</v>
       </c>
       <c r="K94" s="1"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>112</v>
       </c>
@@ -2343,14 +2343,14 @@
         <v>2021</v>
       </c>
       <c r="D95" s="5">
-        <v>49160</v>
+        <v>48835</v>
       </c>
       <c r="E95" s="1">
         <v>1025</v>
       </c>
       <c r="K95" s="1"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>113</v>
       </c>
@@ -2361,13 +2361,13 @@
         <v>2021</v>
       </c>
       <c r="D96" s="5">
-        <v>51335</v>
+        <v>51010</v>
       </c>
       <c r="E96" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>114</v>
       </c>
@@ -2378,13 +2378,13 @@
         <v>2021</v>
       </c>
       <c r="D97" s="5">
-        <v>52090</v>
+        <v>51765</v>
       </c>
       <c r="E97" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>115</v>
       </c>
@@ -2395,13 +2395,13 @@
         <v>2021</v>
       </c>
       <c r="D98" s="5">
-        <v>53700</v>
+        <v>53230</v>
       </c>
       <c r="E98" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B99" t="s">
         <v>122</v>
       </c>

</xml_diff>

<commit_message>
service down test zip updated to 00003
</commit_message>
<xml_diff>
--- a/Data Files/prodMSRPs.xlsx
+++ b/Data Files/prodMSRPs.xlsx
@@ -731,18 +731,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D99" sqref="D99"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D97" sqref="D97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.3984375" customWidth="1"/>
     <col min="2" max="2" width="55" customWidth="1"/>
     <col min="4" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>84</v>
       </c>
@@ -759,7 +759,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>9202</v>
       </c>
@@ -770,13 +770,13 @@
         <v>2021</v>
       </c>
       <c r="D2" s="2">
-        <v>42120</v>
+        <v>42220</v>
       </c>
       <c r="E2" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>9203</v>
       </c>
@@ -787,13 +787,13 @@
         <v>2021</v>
       </c>
       <c r="D3" s="2">
-        <v>46590</v>
+        <v>46690</v>
       </c>
       <c r="E3" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>9206</v>
       </c>
@@ -804,13 +804,13 @@
         <v>2021</v>
       </c>
       <c r="D4" s="2">
-        <v>44810</v>
+        <v>44910</v>
       </c>
       <c r="E4" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>9207</v>
       </c>
@@ -821,13 +821,13 @@
         <v>2021</v>
       </c>
       <c r="D5" s="2">
-        <v>48765</v>
+        <v>48865</v>
       </c>
       <c r="E5" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>9212</v>
       </c>
@@ -838,13 +838,13 @@
         <v>2021</v>
       </c>
       <c r="D6" s="2">
-        <v>45050</v>
+        <v>45150</v>
       </c>
       <c r="E6" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>9213</v>
       </c>
@@ -855,13 +855,13 @@
         <v>2021</v>
       </c>
       <c r="D7" s="2">
-        <v>49520</v>
+        <v>49620</v>
       </c>
       <c r="E7" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>9216</v>
       </c>
@@ -872,13 +872,13 @@
         <v>2021</v>
       </c>
       <c r="D8" s="2">
-        <v>47215</v>
+        <v>47315</v>
       </c>
       <c r="E8" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>9217</v>
       </c>
@@ -889,13 +889,13 @@
         <v>2021</v>
       </c>
       <c r="D9" s="2">
-        <v>51130</v>
+        <v>51230</v>
       </c>
       <c r="E9" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>9000</v>
       </c>
@@ -906,13 +906,13 @@
         <v>2021</v>
       </c>
       <c r="D10" s="2">
-        <v>39900</v>
+        <v>40000</v>
       </c>
       <c r="E10" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>9002</v>
       </c>
@@ -923,13 +923,13 @@
         <v>2021</v>
       </c>
       <c r="D11" s="2">
-        <v>45100</v>
+        <v>45200</v>
       </c>
       <c r="E11" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>9004</v>
       </c>
@@ -940,13 +940,13 @@
         <v>2021</v>
       </c>
       <c r="D12" s="2">
-        <v>48900</v>
+        <v>49000</v>
       </c>
       <c r="E12" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>9040</v>
       </c>
@@ -957,13 +957,13 @@
         <v>2021</v>
       </c>
       <c r="D13" s="2">
-        <v>41810</v>
+        <v>41910</v>
       </c>
       <c r="E13" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>9042</v>
       </c>
@@ -974,13 +974,13 @@
         <v>2021</v>
       </c>
       <c r="D14" s="2">
-        <v>47010</v>
+        <v>47110</v>
       </c>
       <c r="E14" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>9044</v>
       </c>
@@ -991,13 +991,13 @@
         <v>2021</v>
       </c>
       <c r="D15" s="2">
-        <v>50810</v>
+        <v>50910</v>
       </c>
       <c r="E15" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>9005</v>
       </c>
@@ -1008,13 +1008,13 @@
         <v>2021</v>
       </c>
       <c r="D16" s="2">
-        <v>45700</v>
+        <v>45800</v>
       </c>
       <c r="E16" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>9502</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1048,7 +1048,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>9506</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1082,7 +1082,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>9510</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1116,7 +1116,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>9516</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1150,7 +1150,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1164,7 +1164,7 @@
         <v>45200</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1178,7 +1178,7 @@
         <v>47250</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -1192,7 +1192,7 @@
         <v>49415</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -1206,7 +1206,7 @@
         <v>50155</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>9700</v>
       </c>
@@ -1214,16 +1214,16 @@
         <v>32</v>
       </c>
       <c r="C29">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D29" s="2">
-        <v>53100</v>
+        <v>53250</v>
       </c>
       <c r="E29" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -1231,16 +1231,16 @@
         <v>34</v>
       </c>
       <c r="C30">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D30" s="2">
-        <v>55890</v>
+        <v>56340</v>
       </c>
       <c r="E30" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>9710</v>
       </c>
@@ -1248,16 +1248,16 @@
         <v>35</v>
       </c>
       <c r="C31">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D31" s="2">
-        <v>64365</v>
+        <v>64515</v>
       </c>
       <c r="E31" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>9625</v>
       </c>
@@ -1268,13 +1268,13 @@
         <v>2020</v>
       </c>
       <c r="D32" s="2">
-        <v>86580</v>
+        <v>86730</v>
       </c>
       <c r="E32" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>9620</v>
       </c>
@@ -1285,13 +1285,13 @@
         <v>2020</v>
       </c>
       <c r="D33" s="2">
-        <v>91580</v>
+        <v>91730</v>
       </c>
       <c r="E33" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>9820</v>
       </c>
@@ -1319,13 +1319,13 @@
         <v>2021</v>
       </c>
       <c r="D35" s="2">
-        <v>37510</v>
+        <v>37610</v>
       </c>
       <c r="E35" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>9824</v>
       </c>
@@ -1336,13 +1336,13 @@
         <v>2021</v>
       </c>
       <c r="D36" s="2">
-        <v>38910</v>
+        <v>39010</v>
       </c>
       <c r="E36" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>9830</v>
       </c>
@@ -1353,13 +1353,13 @@
         <v>2021</v>
       </c>
       <c r="D37" s="2">
-        <v>39610</v>
+        <v>39710</v>
       </c>
       <c r="E37" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>9834</v>
       </c>
@@ -1370,13 +1370,13 @@
         <v>2021</v>
       </c>
       <c r="D38" s="2">
-        <v>41010</v>
+        <v>41110</v>
       </c>
       <c r="E38" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>9821</v>
       </c>
@@ -1387,13 +1387,13 @@
         <v>2021</v>
       </c>
       <c r="D39" s="2">
-        <v>43960</v>
+        <v>44060</v>
       </c>
       <c r="E39" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>9825</v>
       </c>
@@ -1404,13 +1404,13 @@
         <v>2021</v>
       </c>
       <c r="D40" s="2">
-        <v>45360</v>
+        <v>45460</v>
       </c>
       <c r="E40" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>9844</v>
       </c>
@@ -1421,13 +1421,13 @@
         <v>2021</v>
       </c>
       <c r="D41" s="2">
-        <v>40060</v>
+        <v>40160</v>
       </c>
       <c r="E41" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>9845</v>
       </c>
@@ -1438,13 +1438,13 @@
         <v>2021</v>
       </c>
       <c r="D42" s="2">
-        <v>46510</v>
+        <v>46610</v>
       </c>
       <c r="E42" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>9846</v>
       </c>
@@ -1455,13 +1455,13 @@
         <v>2021</v>
       </c>
       <c r="D43" s="2">
-        <v>46810</v>
+        <v>46910</v>
       </c>
       <c r="E43" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>48</v>
       </c>
@@ -1478,7 +1478,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A45">
         <v>9120</v>
       </c>
@@ -1486,16 +1486,16 @@
         <v>50</v>
       </c>
       <c r="C45">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D45" s="2">
-        <v>75450</v>
+        <v>76000</v>
       </c>
       <c r="E45" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A46">
         <v>9126</v>
       </c>
@@ -1503,16 +1503,16 @@
         <v>51</v>
       </c>
       <c r="C46">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D46" s="2">
-        <v>78670</v>
+        <v>79250</v>
       </c>
       <c r="E46" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A47">
         <v>9122</v>
       </c>
@@ -1520,16 +1520,16 @@
         <v>52</v>
       </c>
       <c r="C47">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D47" s="2">
-        <v>81450</v>
+        <v>79600</v>
       </c>
       <c r="E47" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A48">
         <v>9128</v>
       </c>
@@ -1537,16 +1537,16 @@
         <v>53</v>
       </c>
       <c r="C48">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D48" s="2">
-        <v>84670</v>
+        <v>82850</v>
       </c>
       <c r="E48" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A49">
         <v>9140</v>
       </c>
@@ -1563,7 +1563,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A50">
         <v>9146</v>
       </c>
@@ -1580,7 +1580,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>56</v>
       </c>
@@ -1597,7 +1597,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>56</v>
       </c>
@@ -1614,7 +1614,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A53">
         <v>9225</v>
       </c>
@@ -1625,13 +1625,13 @@
         <v>2021</v>
       </c>
       <c r="D53" s="2">
-        <v>65875</v>
+        <v>65975</v>
       </c>
       <c r="E53" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A54">
         <v>9226</v>
       </c>
@@ -1642,13 +1642,13 @@
         <v>2021</v>
       </c>
       <c r="D54" s="2">
-        <v>97100</v>
+        <v>97625</v>
       </c>
       <c r="E54" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A55">
         <v>9420</v>
       </c>
@@ -1659,13 +1659,13 @@
         <v>2021</v>
       </c>
       <c r="D55" s="2">
-        <v>45070</v>
+        <v>45170</v>
       </c>
       <c r="E55" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A56">
         <v>9424</v>
       </c>
@@ -1676,13 +1676,13 @@
         <v>2021</v>
       </c>
       <c r="D56" s="2">
-        <v>46470</v>
+        <v>46570</v>
       </c>
       <c r="E56" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A57">
         <v>9430</v>
       </c>
@@ -1693,13 +1693,13 @@
         <v>2021</v>
       </c>
       <c r="D57" s="2">
-        <v>47900</v>
+        <v>48000</v>
       </c>
       <c r="E57" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A58">
         <v>9434</v>
       </c>
@@ -1710,13 +1710,13 @@
         <v>2021</v>
       </c>
       <c r="D58" s="2">
-        <v>49300</v>
+        <v>49400</v>
       </c>
       <c r="E58" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A59">
         <v>9422</v>
       </c>
@@ -1727,13 +1727,13 @@
         <v>2021</v>
       </c>
       <c r="D59" s="2">
-        <v>48550</v>
+        <v>48650</v>
       </c>
       <c r="E59" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A60">
         <v>9426</v>
       </c>
@@ -1744,13 +1744,13 @@
         <v>2021</v>
       </c>
       <c r="D60" s="2">
-        <v>49950</v>
+        <v>50050</v>
       </c>
       <c r="E60" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A61">
         <v>9444</v>
       </c>
@@ -1761,13 +1761,13 @@
         <v>2021</v>
       </c>
       <c r="D61" s="2">
-        <v>47720</v>
+        <v>47820</v>
       </c>
       <c r="E61" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A62">
         <v>9454</v>
       </c>
@@ -1778,13 +1778,13 @@
         <v>2021</v>
       </c>
       <c r="D62" s="2">
-        <v>51110</v>
+        <v>51210</v>
       </c>
       <c r="E62" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A63">
         <v>9446</v>
       </c>
@@ -1795,13 +1795,13 @@
         <v>2021</v>
       </c>
       <c r="D63" s="2">
-        <v>51200</v>
+        <v>51300</v>
       </c>
       <c r="E63" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A64">
         <v>9301</v>
       </c>
@@ -1818,7 +1818,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A65">
         <v>9313</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A66">
         <v>9300</v>
       </c>
@@ -1852,7 +1852,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A67">
         <v>9306</v>
       </c>
@@ -1869,7 +1869,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A68">
         <v>9314</v>
       </c>
@@ -1886,7 +1886,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A69">
         <v>9316</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A70">
         <v>9260</v>
       </c>
@@ -1914,13 +1914,13 @@
         <v>2021</v>
       </c>
       <c r="D70" s="2">
-        <v>92950</v>
+        <v>93050</v>
       </c>
       <c r="E70" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A71">
         <v>9264</v>
       </c>
@@ -1931,13 +1931,13 @@
         <v>2021</v>
       </c>
       <c r="D71" s="2">
-        <v>97510</v>
+        <v>97610</v>
       </c>
       <c r="E71" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A72">
         <v>9262</v>
       </c>
@@ -1948,13 +1948,13 @@
         <v>2021</v>
       </c>
       <c r="D72" s="2">
-        <v>101000</v>
+        <v>101100</v>
       </c>
       <c r="E72" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A73">
         <v>9720</v>
       </c>
@@ -1971,7 +1971,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A74">
         <v>9724</v>
       </c>
@@ -1988,7 +1988,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A75">
         <v>9732</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A76">
         <v>9736</v>
       </c>
@@ -2022,7 +2022,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A77">
         <v>9722</v>
       </c>
@@ -2039,7 +2039,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A78">
         <v>9738</v>
       </c>
@@ -2056,7 +2056,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A79">
         <v>9335</v>
       </c>
@@ -2073,7 +2073,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>91</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A81">
         <v>9012</v>
       </c>
@@ -2101,13 +2101,13 @@
         <v>2021</v>
       </c>
       <c r="D81" s="5">
-        <v>39900</v>
+        <v>40000</v>
       </c>
       <c r="E81" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A82">
         <v>9013</v>
       </c>
@@ -2118,13 +2118,13 @@
         <v>2021</v>
       </c>
       <c r="D82" s="5">
-        <v>45100</v>
+        <v>45200</v>
       </c>
       <c r="E82" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A83">
         <v>9014</v>
       </c>
@@ -2135,13 +2135,13 @@
         <v>2021</v>
       </c>
       <c r="D83" s="5">
-        <v>48900</v>
+        <v>49000</v>
       </c>
       <c r="E83" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A84">
         <v>9015</v>
       </c>
@@ -2152,13 +2152,13 @@
         <v>2021</v>
       </c>
       <c r="D84" s="5">
-        <v>45700</v>
+        <v>45800</v>
       </c>
       <c r="E84" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>110</v>
       </c>
@@ -2175,7 +2175,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A86">
         <v>9423</v>
       </c>
@@ -2186,13 +2186,13 @@
         <v>2021</v>
       </c>
       <c r="D86" s="5">
-        <v>50950</v>
+        <v>51050</v>
       </c>
       <c r="E86" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A87">
         <v>9427</v>
       </c>
@@ -2203,13 +2203,13 @@
         <v>2021</v>
       </c>
       <c r="D87" s="5">
-        <v>52350</v>
+        <v>52450</v>
       </c>
       <c r="E87" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A88">
         <v>9447</v>
       </c>
@@ -2220,13 +2220,13 @@
         <v>2021</v>
       </c>
       <c r="D88" s="5">
-        <v>53520</v>
+        <v>53620</v>
       </c>
       <c r="E88" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A89">
         <v>9432</v>
       </c>
@@ -2237,13 +2237,13 @@
         <v>2021</v>
       </c>
       <c r="D89" s="5">
-        <v>53900</v>
+        <v>54000</v>
       </c>
       <c r="E89" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A90">
         <v>9436</v>
       </c>
@@ -2254,13 +2254,13 @@
         <v>2021</v>
       </c>
       <c r="D90" s="5">
-        <v>55300</v>
+        <v>55400</v>
       </c>
       <c r="E90" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A91">
         <v>9457</v>
       </c>
@@ -2271,14 +2271,14 @@
         <v>2021</v>
       </c>
       <c r="D91" s="5">
-        <v>57110</v>
+        <v>57210</v>
       </c>
       <c r="E91" s="1">
         <v>1025</v>
       </c>
       <c r="J91" s="1"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>107</v>
       </c>
@@ -2289,14 +2289,14 @@
         <v>2021</v>
       </c>
       <c r="D92" s="5">
-        <v>49235</v>
+        <v>49335</v>
       </c>
       <c r="E92" s="1">
         <v>1025</v>
       </c>
       <c r="K92" s="1"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>108</v>
       </c>
@@ -2307,14 +2307,14 @@
         <v>2021</v>
       </c>
       <c r="D93" s="5">
-        <v>50635</v>
+        <v>50735</v>
       </c>
       <c r="E93" s="1">
         <v>1025</v>
       </c>
       <c r="K93" s="1"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
         <v>109</v>
       </c>
@@ -2325,14 +2325,14 @@
         <v>2021</v>
       </c>
       <c r="D94" s="5">
-        <v>51885</v>
+        <v>51985</v>
       </c>
       <c r="E94" s="1">
         <v>1025</v>
       </c>
       <c r="K94" s="1"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>112</v>
       </c>
@@ -2343,14 +2343,14 @@
         <v>2021</v>
       </c>
       <c r="D95" s="5">
-        <v>49160</v>
+        <v>48835</v>
       </c>
       <c r="E95" s="1">
         <v>1025</v>
       </c>
       <c r="K95" s="1"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>113</v>
       </c>
@@ -2361,13 +2361,13 @@
         <v>2021</v>
       </c>
       <c r="D96" s="5">
-        <v>51335</v>
+        <v>51010</v>
       </c>
       <c r="E96" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>114</v>
       </c>
@@ -2378,13 +2378,13 @@
         <v>2021</v>
       </c>
       <c r="D97" s="5">
-        <v>52090</v>
+        <v>51765</v>
       </c>
       <c r="E97" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>115</v>
       </c>
@@ -2395,13 +2395,13 @@
         <v>2021</v>
       </c>
       <c r="D98" s="5">
-        <v>53700</v>
+        <v>53230</v>
       </c>
       <c r="E98" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B99" t="s">
         <v>122</v>
       </c>

</xml_diff>

<commit_message>
changed services down test zip to 00003
</commit_message>
<xml_diff>
--- a/Data Files/prodMSRPs.xlsx
+++ b/Data Files/prodMSRPs.xlsx
@@ -731,18 +731,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D97" sqref="D97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.3984375" customWidth="1"/>
     <col min="2" max="2" width="55" customWidth="1"/>
     <col min="4" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>84</v>
       </c>
@@ -759,7 +759,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>9202</v>
       </c>
@@ -770,13 +770,13 @@
         <v>2021</v>
       </c>
       <c r="D2" s="2">
-        <v>42120</v>
+        <v>42220</v>
       </c>
       <c r="E2" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>9203</v>
       </c>
@@ -787,13 +787,13 @@
         <v>2021</v>
       </c>
       <c r="D3" s="2">
-        <v>46590</v>
+        <v>46690</v>
       </c>
       <c r="E3" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>9206</v>
       </c>
@@ -804,13 +804,13 @@
         <v>2021</v>
       </c>
       <c r="D4" s="2">
-        <v>44810</v>
+        <v>44910</v>
       </c>
       <c r="E4" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>9207</v>
       </c>
@@ -821,13 +821,13 @@
         <v>2021</v>
       </c>
       <c r="D5" s="2">
-        <v>48765</v>
+        <v>48865</v>
       </c>
       <c r="E5" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>9212</v>
       </c>
@@ -838,13 +838,13 @@
         <v>2021</v>
       </c>
       <c r="D6" s="2">
-        <v>45050</v>
+        <v>45150</v>
       </c>
       <c r="E6" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>9213</v>
       </c>
@@ -855,13 +855,13 @@
         <v>2021</v>
       </c>
       <c r="D7" s="2">
-        <v>49520</v>
+        <v>49620</v>
       </c>
       <c r="E7" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>9216</v>
       </c>
@@ -872,13 +872,13 @@
         <v>2021</v>
       </c>
       <c r="D8" s="2">
-        <v>47215</v>
+        <v>47315</v>
       </c>
       <c r="E8" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>9217</v>
       </c>
@@ -889,13 +889,13 @@
         <v>2021</v>
       </c>
       <c r="D9" s="2">
-        <v>51130</v>
+        <v>51230</v>
       </c>
       <c r="E9" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>9000</v>
       </c>
@@ -906,13 +906,13 @@
         <v>2021</v>
       </c>
       <c r="D10" s="2">
-        <v>39900</v>
+        <v>40000</v>
       </c>
       <c r="E10" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>9002</v>
       </c>
@@ -923,13 +923,13 @@
         <v>2021</v>
       </c>
       <c r="D11" s="2">
-        <v>45100</v>
+        <v>45200</v>
       </c>
       <c r="E11" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>9004</v>
       </c>
@@ -940,13 +940,13 @@
         <v>2021</v>
       </c>
       <c r="D12" s="2">
-        <v>48900</v>
+        <v>49000</v>
       </c>
       <c r="E12" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>9040</v>
       </c>
@@ -957,13 +957,13 @@
         <v>2021</v>
       </c>
       <c r="D13" s="2">
-        <v>41810</v>
+        <v>41910</v>
       </c>
       <c r="E13" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>9042</v>
       </c>
@@ -974,13 +974,13 @@
         <v>2021</v>
       </c>
       <c r="D14" s="2">
-        <v>47010</v>
+        <v>47110</v>
       </c>
       <c r="E14" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>9044</v>
       </c>
@@ -991,13 +991,13 @@
         <v>2021</v>
       </c>
       <c r="D15" s="2">
-        <v>50810</v>
+        <v>50910</v>
       </c>
       <c r="E15" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>9005</v>
       </c>
@@ -1008,13 +1008,13 @@
         <v>2021</v>
       </c>
       <c r="D16" s="2">
-        <v>45700</v>
+        <v>45800</v>
       </c>
       <c r="E16" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>9502</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1048,7 +1048,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>9506</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1082,7 +1082,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>9510</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1116,7 +1116,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>9516</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1150,7 +1150,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1164,7 +1164,7 @@
         <v>45200</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1178,7 +1178,7 @@
         <v>47250</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -1192,7 +1192,7 @@
         <v>49415</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -1206,7 +1206,7 @@
         <v>50155</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>9700</v>
       </c>
@@ -1217,13 +1217,13 @@
         <v>2021</v>
       </c>
       <c r="D29" s="2">
-        <v>53100</v>
+        <v>53250</v>
       </c>
       <c r="E29" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -1234,13 +1234,13 @@
         <v>2021</v>
       </c>
       <c r="D30" s="2">
-        <v>56190</v>
+        <v>56340</v>
       </c>
       <c r="E30" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>9710</v>
       </c>
@@ -1251,13 +1251,13 @@
         <v>2021</v>
       </c>
       <c r="D31" s="2">
-        <v>64365</v>
+        <v>64515</v>
       </c>
       <c r="E31" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>9625</v>
       </c>
@@ -1268,13 +1268,13 @@
         <v>2020</v>
       </c>
       <c r="D32" s="2">
-        <v>86580</v>
+        <v>86730</v>
       </c>
       <c r="E32" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>9620</v>
       </c>
@@ -1285,13 +1285,13 @@
         <v>2020</v>
       </c>
       <c r="D33" s="2">
-        <v>91580</v>
+        <v>91730</v>
       </c>
       <c r="E33" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>9820</v>
       </c>
@@ -1319,13 +1319,13 @@
         <v>2021</v>
       </c>
       <c r="D35" s="2">
-        <v>37510</v>
+        <v>37610</v>
       </c>
       <c r="E35" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>9824</v>
       </c>
@@ -1336,13 +1336,13 @@
         <v>2021</v>
       </c>
       <c r="D36" s="2">
-        <v>38910</v>
+        <v>39010</v>
       </c>
       <c r="E36" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>9830</v>
       </c>
@@ -1353,13 +1353,13 @@
         <v>2021</v>
       </c>
       <c r="D37" s="2">
-        <v>39610</v>
+        <v>39710</v>
       </c>
       <c r="E37" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>9834</v>
       </c>
@@ -1370,13 +1370,13 @@
         <v>2021</v>
       </c>
       <c r="D38" s="2">
-        <v>41010</v>
+        <v>41110</v>
       </c>
       <c r="E38" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>9821</v>
       </c>
@@ -1387,13 +1387,13 @@
         <v>2021</v>
       </c>
       <c r="D39" s="2">
-        <v>43960</v>
+        <v>44060</v>
       </c>
       <c r="E39" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>9825</v>
       </c>
@@ -1404,13 +1404,13 @@
         <v>2021</v>
       </c>
       <c r="D40" s="2">
-        <v>45360</v>
+        <v>45460</v>
       </c>
       <c r="E40" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>9844</v>
       </c>
@@ -1421,13 +1421,13 @@
         <v>2021</v>
       </c>
       <c r="D41" s="2">
-        <v>40060</v>
+        <v>40160</v>
       </c>
       <c r="E41" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>9845</v>
       </c>
@@ -1438,13 +1438,13 @@
         <v>2021</v>
       </c>
       <c r="D42" s="2">
-        <v>46510</v>
+        <v>46610</v>
       </c>
       <c r="E42" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>9846</v>
       </c>
@@ -1455,13 +1455,13 @@
         <v>2021</v>
       </c>
       <c r="D43" s="2">
-        <v>46810</v>
+        <v>46910</v>
       </c>
       <c r="E43" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>48</v>
       </c>
@@ -1478,7 +1478,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A45">
         <v>9120</v>
       </c>
@@ -1486,16 +1486,16 @@
         <v>50</v>
       </c>
       <c r="C45">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D45" s="2">
-        <v>75450</v>
+        <v>76000</v>
       </c>
       <c r="E45" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A46">
         <v>9126</v>
       </c>
@@ -1503,16 +1503,16 @@
         <v>51</v>
       </c>
       <c r="C46">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D46" s="2">
-        <v>78670</v>
+        <v>79250</v>
       </c>
       <c r="E46" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A47">
         <v>9122</v>
       </c>
@@ -1520,16 +1520,16 @@
         <v>52</v>
       </c>
       <c r="C47">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D47" s="2">
-        <v>81450</v>
+        <v>79600</v>
       </c>
       <c r="E47" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A48">
         <v>9128</v>
       </c>
@@ -1537,16 +1537,16 @@
         <v>53</v>
       </c>
       <c r="C48">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D48" s="2">
-        <v>84670</v>
+        <v>82850</v>
       </c>
       <c r="E48" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A49">
         <v>9140</v>
       </c>
@@ -1563,7 +1563,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A50">
         <v>9146</v>
       </c>
@@ -1580,7 +1580,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>56</v>
       </c>
@@ -1597,7 +1597,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>56</v>
       </c>
@@ -1614,7 +1614,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A53">
         <v>9225</v>
       </c>
@@ -1625,13 +1625,13 @@
         <v>2021</v>
       </c>
       <c r="D53" s="2">
-        <v>65875</v>
+        <v>65975</v>
       </c>
       <c r="E53" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A54">
         <v>9226</v>
       </c>
@@ -1642,13 +1642,13 @@
         <v>2021</v>
       </c>
       <c r="D54" s="2">
-        <v>97100</v>
+        <v>97625</v>
       </c>
       <c r="E54" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A55">
         <v>9420</v>
       </c>
@@ -1659,13 +1659,13 @@
         <v>2021</v>
       </c>
       <c r="D55" s="2">
-        <v>45070</v>
+        <v>45170</v>
       </c>
       <c r="E55" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A56">
         <v>9424</v>
       </c>
@@ -1676,13 +1676,13 @@
         <v>2021</v>
       </c>
       <c r="D56" s="2">
-        <v>46470</v>
+        <v>46570</v>
       </c>
       <c r="E56" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A57">
         <v>9430</v>
       </c>
@@ -1693,13 +1693,13 @@
         <v>2021</v>
       </c>
       <c r="D57" s="2">
-        <v>47900</v>
+        <v>48000</v>
       </c>
       <c r="E57" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A58">
         <v>9434</v>
       </c>
@@ -1710,13 +1710,13 @@
         <v>2021</v>
       </c>
       <c r="D58" s="2">
-        <v>49300</v>
+        <v>49400</v>
       </c>
       <c r="E58" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A59">
         <v>9422</v>
       </c>
@@ -1727,13 +1727,13 @@
         <v>2021</v>
       </c>
       <c r="D59" s="2">
-        <v>48550</v>
+        <v>48650</v>
       </c>
       <c r="E59" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A60">
         <v>9426</v>
       </c>
@@ -1744,13 +1744,13 @@
         <v>2021</v>
       </c>
       <c r="D60" s="2">
-        <v>49950</v>
+        <v>50050</v>
       </c>
       <c r="E60" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A61">
         <v>9444</v>
       </c>
@@ -1761,13 +1761,13 @@
         <v>2021</v>
       </c>
       <c r="D61" s="2">
-        <v>47720</v>
+        <v>47820</v>
       </c>
       <c r="E61" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A62">
         <v>9454</v>
       </c>
@@ -1778,13 +1778,13 @@
         <v>2021</v>
       </c>
       <c r="D62" s="2">
-        <v>51110</v>
+        <v>51210</v>
       </c>
       <c r="E62" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A63">
         <v>9446</v>
       </c>
@@ -1795,13 +1795,13 @@
         <v>2021</v>
       </c>
       <c r="D63" s="2">
-        <v>51200</v>
+        <v>51300</v>
       </c>
       <c r="E63" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A64">
         <v>9301</v>
       </c>
@@ -1818,7 +1818,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A65">
         <v>9313</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A66">
         <v>9300</v>
       </c>
@@ -1852,7 +1852,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A67">
         <v>9306</v>
       </c>
@@ -1869,7 +1869,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A68">
         <v>9314</v>
       </c>
@@ -1886,7 +1886,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A69">
         <v>9316</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A70">
         <v>9260</v>
       </c>
@@ -1914,13 +1914,13 @@
         <v>2021</v>
       </c>
       <c r="D70" s="2">
-        <v>92950</v>
+        <v>93050</v>
       </c>
       <c r="E70" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A71">
         <v>9264</v>
       </c>
@@ -1931,13 +1931,13 @@
         <v>2021</v>
       </c>
       <c r="D71" s="2">
-        <v>97510</v>
+        <v>97610</v>
       </c>
       <c r="E71" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A72">
         <v>9262</v>
       </c>
@@ -1948,13 +1948,13 @@
         <v>2021</v>
       </c>
       <c r="D72" s="2">
-        <v>101000</v>
+        <v>101100</v>
       </c>
       <c r="E72" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A73">
         <v>9720</v>
       </c>
@@ -1971,7 +1971,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A74">
         <v>9724</v>
       </c>
@@ -1988,7 +1988,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A75">
         <v>9732</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A76">
         <v>9736</v>
       </c>
@@ -2022,7 +2022,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A77">
         <v>9722</v>
       </c>
@@ -2039,7 +2039,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A78">
         <v>9738</v>
       </c>
@@ -2056,7 +2056,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A79">
         <v>9335</v>
       </c>
@@ -2073,7 +2073,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>91</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A81">
         <v>9012</v>
       </c>
@@ -2101,13 +2101,13 @@
         <v>2021</v>
       </c>
       <c r="D81" s="5">
-        <v>39900</v>
+        <v>40000</v>
       </c>
       <c r="E81" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A82">
         <v>9013</v>
       </c>
@@ -2118,13 +2118,13 @@
         <v>2021</v>
       </c>
       <c r="D82" s="5">
-        <v>45100</v>
+        <v>45200</v>
       </c>
       <c r="E82" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A83">
         <v>9014</v>
       </c>
@@ -2135,13 +2135,13 @@
         <v>2021</v>
       </c>
       <c r="D83" s="5">
-        <v>48900</v>
+        <v>49000</v>
       </c>
       <c r="E83" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A84">
         <v>9015</v>
       </c>
@@ -2152,13 +2152,13 @@
         <v>2021</v>
       </c>
       <c r="D84" s="5">
-        <v>45700</v>
+        <v>45800</v>
       </c>
       <c r="E84" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>110</v>
       </c>
@@ -2175,7 +2175,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A86">
         <v>9423</v>
       </c>
@@ -2186,13 +2186,13 @@
         <v>2021</v>
       </c>
       <c r="D86" s="5">
-        <v>50950</v>
+        <v>51050</v>
       </c>
       <c r="E86" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A87">
         <v>9427</v>
       </c>
@@ -2203,13 +2203,13 @@
         <v>2021</v>
       </c>
       <c r="D87" s="5">
-        <v>52350</v>
+        <v>52450</v>
       </c>
       <c r="E87" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A88">
         <v>9447</v>
       </c>
@@ -2220,13 +2220,13 @@
         <v>2021</v>
       </c>
       <c r="D88" s="5">
-        <v>53520</v>
+        <v>53620</v>
       </c>
       <c r="E88" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A89">
         <v>9432</v>
       </c>
@@ -2237,13 +2237,13 @@
         <v>2021</v>
       </c>
       <c r="D89" s="5">
-        <v>53900</v>
+        <v>54000</v>
       </c>
       <c r="E89" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A90">
         <v>9436</v>
       </c>
@@ -2254,13 +2254,13 @@
         <v>2021</v>
       </c>
       <c r="D90" s="5">
-        <v>55300</v>
+        <v>55400</v>
       </c>
       <c r="E90" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A91">
         <v>9457</v>
       </c>
@@ -2271,14 +2271,14 @@
         <v>2021</v>
       </c>
       <c r="D91" s="5">
-        <v>57110</v>
+        <v>57210</v>
       </c>
       <c r="E91" s="1">
         <v>1025</v>
       </c>
       <c r="J91" s="1"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>107</v>
       </c>
@@ -2289,14 +2289,14 @@
         <v>2021</v>
       </c>
       <c r="D92" s="5">
-        <v>49235</v>
+        <v>49335</v>
       </c>
       <c r="E92" s="1">
         <v>1025</v>
       </c>
       <c r="K92" s="1"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>108</v>
       </c>
@@ -2307,14 +2307,14 @@
         <v>2021</v>
       </c>
       <c r="D93" s="5">
-        <v>50635</v>
+        <v>50735</v>
       </c>
       <c r="E93" s="1">
         <v>1025</v>
       </c>
       <c r="K93" s="1"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
         <v>109</v>
       </c>
@@ -2325,14 +2325,14 @@
         <v>2021</v>
       </c>
       <c r="D94" s="5">
-        <v>51885</v>
+        <v>51985</v>
       </c>
       <c r="E94" s="1">
         <v>1025</v>
       </c>
       <c r="K94" s="1"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>112</v>
       </c>
@@ -2343,14 +2343,14 @@
         <v>2021</v>
       </c>
       <c r="D95" s="5">
-        <v>49160</v>
+        <v>48835</v>
       </c>
       <c r="E95" s="1">
         <v>1025</v>
       </c>
       <c r="K95" s="1"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>113</v>
       </c>
@@ -2361,13 +2361,13 @@
         <v>2021</v>
       </c>
       <c r="D96" s="5">
-        <v>51335</v>
+        <v>51010</v>
       </c>
       <c r="E96" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>114</v>
       </c>
@@ -2378,13 +2378,13 @@
         <v>2021</v>
       </c>
       <c r="D97" s="5">
-        <v>52090</v>
+        <v>51765</v>
       </c>
       <c r="E97" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>115</v>
       </c>
@@ -2395,13 +2395,13 @@
         <v>2021</v>
       </c>
       <c r="D98" s="5">
-        <v>53700</v>
+        <v>53230</v>
       </c>
       <c r="E98" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B99" t="s">
         <v>122</v>
       </c>

</xml_diff>

<commit_message>
LSh enabled on prod
</commit_message>
<xml_diff>
--- a/Data Files/prodMSRPs.xlsx
+++ b/Data Files/prodMSRPs.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="126">
   <si>
     <t>RC 300 RWD</t>
   </si>
@@ -396,6 +396,12 @@
   </si>
   <si>
     <t>COMING SOON</t>
+  </si>
+  <si>
+    <t>LC 500 INSPIRATION SERIES</t>
+  </si>
+  <si>
+    <t>9260LE</t>
   </si>
 </sst>
 </file>
@@ -729,10 +735,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K99"/>
+  <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D97" sqref="D97"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D73" sqref="D73:D78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1554,10 +1560,10 @@
         <v>54</v>
       </c>
       <c r="C49">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D49" s="2">
-        <v>80010</v>
+        <v>90500</v>
       </c>
       <c r="E49" s="1">
         <v>1025</v>
@@ -1571,10 +1577,10 @@
         <v>55</v>
       </c>
       <c r="C50">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D50" s="2">
-        <v>83230</v>
+        <v>93750</v>
       </c>
       <c r="E50" s="1">
         <v>1025</v>
@@ -1965,7 +1971,7 @@
         <v>2021</v>
       </c>
       <c r="D73" s="3">
-        <v>32900</v>
+        <v>33000</v>
       </c>
       <c r="E73" s="1">
         <v>1025</v>
@@ -1982,7 +1988,7 @@
         <v>2021</v>
       </c>
       <c r="D74" s="3">
-        <v>37600</v>
+        <v>37700</v>
       </c>
       <c r="E74" s="1">
         <v>1025</v>
@@ -1999,7 +2005,7 @@
         <v>2021</v>
       </c>
       <c r="D75" s="3">
-        <v>35100</v>
+        <v>35200</v>
       </c>
       <c r="E75" s="1">
         <v>1025</v>
@@ -2016,7 +2022,7 @@
         <v>2021</v>
       </c>
       <c r="D76" s="3">
-        <v>39800</v>
+        <v>39900</v>
       </c>
       <c r="E76" s="1">
         <v>1025</v>
@@ -2033,7 +2039,7 @@
         <v>2021</v>
       </c>
       <c r="D77" s="3">
-        <v>34900</v>
+        <v>35000</v>
       </c>
       <c r="E77" s="1">
         <v>1025</v>
@@ -2050,7 +2056,7 @@
         <v>2021</v>
       </c>
       <c r="D78" s="3">
-        <v>37100</v>
+        <v>37200</v>
       </c>
       <c r="E78" s="1">
         <v>1025</v>
@@ -2084,7 +2090,7 @@
         <v>2021</v>
       </c>
       <c r="D80" s="2">
-        <v>119800</v>
+        <v>119900</v>
       </c>
       <c r="E80" s="1">
         <v>1025</v>
@@ -2412,6 +2418,23 @@
         <v>123</v>
       </c>
       <c r="E99" s="1">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A100" t="s">
+        <v>125</v>
+      </c>
+      <c r="B100" t="s">
+        <v>124</v>
+      </c>
+      <c r="C100">
+        <v>2021</v>
+      </c>
+      <c r="D100" s="2">
+        <v>110420</v>
+      </c>
+      <c r="E100" s="1">
         <v>1025</v>
       </c>
     </row>

</xml_diff>